<commit_message>
Update: Add parts mapping image
</commit_message>
<xml_diff>
--- a/fabrication/elecrow/CO60-PCBA-Quotation.xlsx
+++ b/fabrication/elecrow/CO60-PCBA-Quotation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PCB Specification" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="323">
   <si>
     <t xml:space="preserve">Your PCB Specification</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t xml:space="preserve">C137619</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5% tolerance or less</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.mouser.ca/datasheet/2/427/mcx0x0xpro-223600.pdf</t>
@@ -1335,7 +1338,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -1343,14 +1346,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>436680</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>65160</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>388440</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" descr=""/>
+        <xdr:cNvPr id="0" name="Image 1" descr="Picture generated by PCBNEW "/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1360,7 +1363,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="15238440" cy="9380520"/>
+          <a:ext cx="12370680" cy="4391280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1388,10 +1391,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="7.92712550607287"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="26" min="6" style="0" width="7.92712550607287"/>
     <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.57085020242915"/>
   </cols>
@@ -1566,8 +1569,8 @@
   </sheetPr>
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L22" activeCellId="0" sqref="L22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1575,14 +1578,14 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.82186234817814"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.92712550607287"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.2793522267206"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="10" min="9" style="0" width="7.92712550607287"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="26" min="15" style="0" width="7.92712550607287"/>
     <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.57085020242915"/>
   </cols>
@@ -2116,9 +2119,11 @@
       <c r="L11" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="M11" s="9"/>
+      <c r="M11" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="N11" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
@@ -2138,19 +2143,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C12" s="11" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>39</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>88</v>
@@ -2164,11 +2169,13 @@
       </c>
       <c r="K12" s="8"/>
       <c r="L12" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="M12" s="9"/>
+        <v>95</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="N12" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
@@ -2188,7 +2195,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C13" s="11" t="n">
         <v>2</v>
@@ -2200,7 +2207,7 @@
         <v>39</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>88</v>
@@ -2214,11 +2221,13 @@
       </c>
       <c r="K13" s="8"/>
       <c r="L13" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="M13" s="9"/>
+        <v>99</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="N13" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
@@ -2238,19 +2247,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C14" s="11" t="n">
         <v>2</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>39</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>88</v>
@@ -2264,11 +2273,13 @@
       </c>
       <c r="K14" s="8"/>
       <c r="L14" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="M14" s="9"/>
+        <v>104</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="N14" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="O14" s="9"/>
       <c r="P14" s="9"/>
@@ -2288,22 +2299,22 @@
         <v>13</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C15" s="11" t="n">
         <v>16</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E15" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>106</v>
-      </c>
       <c r="G15" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H15" s="8" t="n">
         <v>64</v>
@@ -2314,11 +2325,11 @@
       </c>
       <c r="K15" s="8"/>
       <c r="L15" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M15" s="9"/>
       <c r="N15" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="O15" s="9"/>
       <c r="P15" s="9"/>
@@ -2338,22 +2349,22 @@
         <v>14</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C16" s="11" t="n">
         <v>1</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H16" s="8" t="n">
         <v>4</v>
@@ -2364,11 +2375,11 @@
       </c>
       <c r="K16" s="8"/>
       <c r="L16" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M16" s="9"/>
       <c r="N16" s="10" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
@@ -2388,22 +2399,22 @@
         <v>15</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C17" s="11" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E17" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>119</v>
-      </c>
       <c r="G17" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H17" s="8" t="n">
         <v>5</v>
@@ -2414,11 +2425,11 @@
       </c>
       <c r="K17" s="8"/>
       <c r="L17" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="M17" s="9"/>
       <c r="N17" s="15" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O17" s="13"/>
       <c r="P17" s="13"/>
@@ -2438,22 +2449,22 @@
         <v>16</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C18" s="11" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E18" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="F18" s="10" t="s">
-        <v>125</v>
-      </c>
       <c r="G18" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H18" s="8" t="n">
         <v>6</v>
@@ -2464,11 +2475,11 @@
       </c>
       <c r="K18" s="8"/>
       <c r="L18" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="M18" s="9"/>
       <c r="N18" s="10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O18" s="13"/>
       <c r="P18" s="13"/>
@@ -2488,22 +2499,22 @@
         <v>17</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C19" s="11" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E19" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="F19" s="10" t="s">
-        <v>131</v>
-      </c>
       <c r="G19" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H19" s="8" t="n">
         <v>48</v>
@@ -2514,11 +2525,11 @@
       </c>
       <c r="K19" s="8"/>
       <c r="L19" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="M19" s="9"/>
       <c r="N19" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="O19" s="13"/>
       <c r="P19" s="13"/>
@@ -2538,22 +2549,22 @@
         <v>18</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C20" s="11" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E20" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="F20" s="10" t="s">
-        <v>137</v>
-      </c>
       <c r="G20" s="13" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H20" s="8" t="n">
         <v>5</v>
@@ -2564,11 +2575,11 @@
       </c>
       <c r="K20" s="8"/>
       <c r="L20" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="M20" s="9"/>
       <c r="N20" s="10" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O20" s="13"/>
       <c r="P20" s="13"/>
@@ -2588,22 +2599,22 @@
         <v>19</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C21" s="11" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E21" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F21" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="F21" s="10" t="s">
-        <v>143</v>
-      </c>
       <c r="G21" s="13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H21" s="8" t="n">
         <v>12</v>
@@ -2614,11 +2625,11 @@
       </c>
       <c r="K21" s="8"/>
       <c r="L21" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="M21" s="9"/>
       <c r="N21" s="10" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="O21" s="13"/>
       <c r="P21" s="13"/>
@@ -2638,22 +2649,22 @@
         <v>20</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C22" s="11" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H22" s="8" t="n">
         <v>4</v>
@@ -2664,11 +2675,11 @@
       </c>
       <c r="K22" s="8"/>
       <c r="L22" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M22" s="9"/>
       <c r="N22" s="10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="O22" s="13"/>
       <c r="P22" s="13"/>
@@ -2691,7 +2702,7 @@
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
       <c r="G23" s="17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H23" s="17" t="n">
         <f aca="false">SUM(H3:H22)</f>
@@ -2750,7 +2761,7 @@
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="16"/>
       <c r="B25" s="19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
@@ -2780,7 +2791,7 @@
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="16"/>
       <c r="B26" s="19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -2831,11 +2842,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="26" min="1" style="0" width="7.92712550607287"/>
     <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.57085020242915"/>
@@ -2870,40 +2881,40 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="26" min="6" style="0" width="7.92712550607287"/>
     <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C2" s="11" t="n">
         <v>45.5614</v>
@@ -2912,7 +2923,7 @@
         <v>56.88</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F2" s="11" t="n">
         <v>180</v>
@@ -2920,10 +2931,10 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C3" s="11" t="n">
         <v>45.5422</v>
@@ -2932,7 +2943,7 @@
         <v>61.62</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F3" s="11" t="n">
         <v>0</v>
@@ -2940,10 +2951,10 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C4" s="11" t="n">
         <v>30.5689</v>
@@ -2952,7 +2963,7 @@
         <v>62.7856</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F4" s="11" t="n">
         <v>90</v>
@@ -2960,10 +2971,10 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C5" s="11" t="n">
         <v>38.6334</v>
@@ -2972,7 +2983,7 @@
         <v>55.88</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F5" s="11" t="n">
         <v>0</v>
@@ -2983,7 +2994,7 @@
         <v>61</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C6" s="11" t="n">
         <v>19.8533</v>
@@ -2992,7 +3003,7 @@
         <v>55.6419</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F6" s="11" t="n">
         <v>270</v>
@@ -3000,10 +3011,10 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C7" s="11" t="n">
         <v>19.8533</v>
@@ -3012,7 +3023,7 @@
         <v>49.6887</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F7" s="11" t="n">
         <v>180</v>
@@ -3023,7 +3034,7 @@
         <v>46</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C8" s="11" t="n">
         <v>35.2814</v>
@@ -3032,7 +3043,7 @@
         <v>45.02</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F8" s="11" t="n">
         <v>0</v>
@@ -3040,10 +3051,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C9" s="11" t="n">
         <v>19.8533</v>
@@ -3052,7 +3063,7 @@
         <v>59.2137</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F9" s="11" t="n">
         <v>180</v>
@@ -3060,10 +3071,10 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C10" s="11" t="n">
         <v>5.8674</v>
@@ -3072,7 +3083,7 @@
         <v>91.44</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F10" s="11" t="n">
         <v>0</v>
@@ -3080,10 +3091,10 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C11" s="11" t="n">
         <v>36.522</v>
@@ -3092,7 +3103,7 @@
         <v>86.5981</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F11" s="11" t="n">
         <v>90</v>
@@ -3100,10 +3111,10 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C12" s="11" t="n">
         <v>55.572</v>
@@ -3112,7 +3123,7 @@
         <v>86.5981</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F12" s="11" t="n">
         <v>90</v>
@@ -3120,10 +3131,10 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C13" s="11" t="n">
         <v>74.7814</v>
@@ -3132,7 +3143,7 @@
         <v>88.93</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F13" s="11" t="n">
         <v>180</v>
@@ -3140,10 +3151,10 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C14" s="11" t="n">
         <v>93.672</v>
@@ -3152,7 +3163,7 @@
         <v>86.5981</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F14" s="11" t="n">
         <v>90</v>
@@ -3160,10 +3171,10 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C15" s="11" t="n">
         <v>112.722</v>
@@ -3172,7 +3183,7 @@
         <v>86.5981</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F15" s="11" t="n">
         <v>90</v>
@@ -3180,10 +3191,10 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C16" s="11" t="n">
         <v>131.772</v>
@@ -3192,7 +3203,7 @@
         <v>86.5981</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F16" s="11" t="n">
         <v>90</v>
@@ -3200,10 +3211,10 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C17" s="11" t="n">
         <v>150.822</v>
@@ -3212,7 +3223,7 @@
         <v>86.5981</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F17" s="11" t="n">
         <v>90</v>
@@ -3220,10 +3231,10 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C18" s="11" t="n">
         <v>169.872</v>
@@ -3232,7 +3243,7 @@
         <v>86.5981</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F18" s="11" t="n">
         <v>90</v>
@@ -3240,10 +3251,10 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C19" s="11" t="n">
         <v>188.7714</v>
@@ -3252,7 +3263,7 @@
         <v>88.85</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F19" s="11" t="n">
         <v>180</v>
@@ -3260,10 +3271,10 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C20" s="11" t="n">
         <v>207.972</v>
@@ -3272,7 +3283,7 @@
         <v>86.5981</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F20" s="11" t="n">
         <v>90</v>
@@ -3280,10 +3291,10 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C21" s="11" t="n">
         <v>227.022</v>
@@ -3292,7 +3303,7 @@
         <v>86.5981</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F21" s="11" t="n">
         <v>90</v>
@@ -3300,10 +3311,10 @@
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C22" s="11" t="n">
         <v>246.072</v>
@@ -3312,7 +3323,7 @@
         <v>86.5981</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F22" s="11" t="n">
         <v>90</v>
@@ -3320,10 +3331,10 @@
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C23" s="11" t="n">
         <v>265.7094</v>
@@ -3332,7 +3343,7 @@
         <v>90.17</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F23" s="11" t="n">
         <v>90</v>
@@ -3340,10 +3351,10 @@
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C24" s="11" t="n">
         <v>281.7908</v>
@@ -3352,7 +3363,7 @@
         <v>90.17</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F24" s="11" t="n">
         <v>90</v>
@@ -3360,10 +3371,10 @@
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C25" s="11" t="n">
         <v>5.5658</v>
@@ -3372,7 +3383,7 @@
         <v>71.12</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F25" s="11" t="n">
         <v>90</v>
@@ -3380,10 +3391,10 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C26" s="11" t="n">
         <v>46.047</v>
@@ -3392,7 +3403,7 @@
         <v>67.5481</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F26" s="11" t="n">
         <v>90</v>
@@ -3400,10 +3411,10 @@
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C27" s="11" t="n">
         <v>65.097</v>
@@ -3412,7 +3423,7 @@
         <v>67.5481</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F27" s="11" t="n">
         <v>90</v>
@@ -3420,10 +3431,10 @@
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C28" s="11" t="n">
         <v>84.147</v>
@@ -3432,7 +3443,7 @@
         <v>67.5481</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F28" s="11" t="n">
         <v>90</v>
@@ -3440,10 +3451,10 @@
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C29" s="11" t="n">
         <v>103.197</v>
@@ -3452,7 +3463,7 @@
         <v>67.5481</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F29" s="11" t="n">
         <v>90</v>
@@ -3460,10 +3471,10 @@
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C30" s="11" t="n">
         <v>122.247</v>
@@ -3472,7 +3483,7 @@
         <v>67.5481</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F30" s="11" t="n">
         <v>90</v>
@@ -3480,10 +3491,10 @@
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C31" s="11" t="n">
         <v>141.297</v>
@@ -3492,7 +3503,7 @@
         <v>67.5481</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F31" s="11" t="n">
         <v>90</v>
@@ -3500,10 +3511,10 @@
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C32" s="11" t="n">
         <v>160.347</v>
@@ -3512,7 +3523,7 @@
         <v>67.5481</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F32" s="11" t="n">
         <v>90</v>
@@ -3520,10 +3531,10 @@
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C33" s="11" t="n">
         <v>179.397</v>
@@ -3532,7 +3543,7 @@
         <v>67.5481</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F33" s="11" t="n">
         <v>90</v>
@@ -3540,10 +3551,10 @@
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C34" s="11" t="n">
         <v>198.447</v>
@@ -3552,7 +3563,7 @@
         <v>67.5481</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F34" s="11" t="n">
         <v>90</v>
@@ -3560,10 +3571,10 @@
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C35" s="11" t="n">
         <v>217.497</v>
@@ -3572,7 +3583,7 @@
         <v>67.5481</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F35" s="11" t="n">
         <v>90</v>
@@ -3580,10 +3591,10 @@
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C36" s="11" t="n">
         <v>236.547</v>
@@ -3592,7 +3603,7 @@
         <v>67.5481</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F36" s="11" t="n">
         <v>90</v>
@@ -3600,10 +3611,10 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C37" s="11" t="n">
         <v>254.4064</v>
@@ -3612,7 +3623,7 @@
         <v>69.9294</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F37" s="11" t="n">
         <v>90</v>
@@ -3620,10 +3631,10 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C38" s="11" t="n">
         <v>277.0283</v>
@@ -3632,7 +3643,7 @@
         <v>71.12</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F38" s="11" t="n">
         <v>90</v>
@@ -3640,10 +3651,10 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C39" s="11" t="n">
         <v>21.0439</v>
@@ -3652,7 +3663,7 @@
         <v>42.545</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F39" s="11" t="n">
         <v>90</v>
@@ -3660,10 +3671,10 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C40" s="11" t="n">
         <v>50.8095</v>
@@ -3672,7 +3683,7 @@
         <v>48.4981</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F40" s="11" t="n">
         <v>90</v>
@@ -3680,10 +3691,10 @@
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C41" s="11" t="n">
         <v>69.8595</v>
@@ -3692,7 +3703,7 @@
         <v>48.4981</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F41" s="11" t="n">
         <v>90</v>
@@ -3700,10 +3711,10 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C42" s="11" t="n">
         <v>88.9095</v>
@@ -3712,7 +3723,7 @@
         <v>48.4981</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F42" s="11" t="n">
         <v>90</v>
@@ -3720,10 +3731,10 @@
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C43" s="11" t="n">
         <v>107.9595</v>
@@ -3732,7 +3743,7 @@
         <v>48.4981</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F43" s="11" t="n">
         <v>90</v>
@@ -3740,10 +3751,10 @@
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C44" s="11" t="n">
         <v>110.8329</v>
@@ -3752,7 +3763,7 @@
         <v>48.5003</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F44" s="11" t="n">
         <v>90</v>
@@ -3760,10 +3771,10 @@
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C45" s="11" t="n">
         <v>146.0595</v>
@@ -3772,7 +3783,7 @@
         <v>48.4981</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F45" s="11" t="n">
         <v>90</v>
@@ -3780,10 +3791,10 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C46" s="11" t="n">
         <v>165.1095</v>
@@ -3792,7 +3803,7 @@
         <v>48.4981</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F46" s="11" t="n">
         <v>90</v>
@@ -3800,10 +3811,10 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C47" s="11" t="n">
         <v>184.1595</v>
@@ -3812,7 +3823,7 @@
         <v>48.4981</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F47" s="11" t="n">
         <v>90</v>
@@ -3820,10 +3831,10 @@
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C48" s="11" t="n">
         <v>203.2095</v>
@@ -3832,7 +3843,7 @@
         <v>48.4981</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F48" s="11" t="n">
         <v>90</v>
@@ -3840,10 +3851,10 @@
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C49" s="11" t="n">
         <v>222.2595</v>
@@ -3852,7 +3863,7 @@
         <v>48.4981</v>
       </c>
       <c r="E49" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F49" s="11" t="n">
         <v>90</v>
@@ -3860,10 +3871,10 @@
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C50" s="11" t="n">
         <v>241.3095</v>
@@ -3872,7 +3883,7 @@
         <v>48.4981</v>
       </c>
       <c r="E50" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F50" s="11" t="n">
         <v>90</v>
@@ -3880,10 +3891,10 @@
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C51" s="11" t="n">
         <v>259.1689</v>
@@ -3892,7 +3903,7 @@
         <v>54.4512</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F51" s="11" t="n">
         <v>90</v>
@@ -3900,10 +3911,10 @@
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C52" s="11" t="n">
         <v>272.2658</v>
@@ -3912,7 +3923,7 @@
         <v>47.3075</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F52" s="11" t="n">
         <v>90</v>
@@ -3920,10 +3931,10 @@
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C53" s="11" t="n">
         <v>3.1845</v>
@@ -3932,7 +3943,7 @@
         <v>29.4481</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F53" s="11" t="n">
         <v>90</v>
@@ -3940,10 +3951,10 @@
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C54" s="11" t="n">
         <v>41.2845</v>
@@ -3952,7 +3963,7 @@
         <v>29.4481</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F54" s="11" t="n">
         <v>90</v>
@@ -3960,10 +3971,10 @@
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C55" s="11" t="n">
         <v>60.3345</v>
@@ -3972,7 +3983,7 @@
         <v>29.4481</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F55" s="11" t="n">
         <v>90</v>
@@ -3980,10 +3991,10 @@
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C56" s="11" t="n">
         <v>79.3845</v>
@@ -3992,7 +4003,7 @@
         <v>29.4481</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F56" s="11" t="n">
         <v>90</v>
@@ -4000,10 +4011,10 @@
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="9" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C57" s="11" t="n">
         <v>98.4345</v>
@@ -4012,7 +4023,7 @@
         <v>29.4481</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F57" s="11" t="n">
         <v>90</v>
@@ -4020,10 +4031,10 @@
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="9" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C58" s="11" t="n">
         <v>117.4845</v>
@@ -4032,7 +4043,7 @@
         <v>29.4481</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F58" s="11" t="n">
         <v>90</v>
@@ -4040,10 +4051,10 @@
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="9" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C59" s="11" t="n">
         <v>136.5345</v>
@@ -4052,7 +4063,7 @@
         <v>29.4481</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F59" s="11" t="n">
         <v>90</v>
@@ -4060,10 +4071,10 @@
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="9" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C60" s="11" t="n">
         <v>155.5845</v>
@@ -4072,7 +4083,7 @@
         <v>29.4481</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F60" s="11" t="n">
         <v>90</v>
@@ -4080,10 +4091,10 @@
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C61" s="11" t="n">
         <v>174.6345</v>
@@ -4092,7 +4103,7 @@
         <v>29.4481</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F61" s="11" t="n">
         <v>90</v>
@@ -4100,10 +4111,10 @@
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C62" s="11" t="n">
         <v>193.6845</v>
@@ -4112,7 +4123,7 @@
         <v>29.4481</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F62" s="11" t="n">
         <v>90</v>
@@ -4120,10 +4131,10 @@
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C63" s="11" t="n">
         <v>212.7345</v>
@@ -4132,7 +4143,7 @@
         <v>29.4481</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F63" s="11" t="n">
         <v>90</v>
@@ -4140,10 +4151,10 @@
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="9" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C64" s="11" t="n">
         <v>231.7845</v>
@@ -4152,7 +4163,7 @@
         <v>29.4481</v>
       </c>
       <c r="E64" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F64" s="11" t="n">
         <v>90</v>
@@ -4160,10 +4171,10 @@
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C65" s="11" t="n">
         <v>267.5033</v>
@@ -4172,7 +4183,7 @@
         <v>29.4481</v>
       </c>
       <c r="E65" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F65" s="11" t="n">
         <v>90</v>
@@ -4180,10 +4191,10 @@
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C66" s="11" t="n">
         <v>281.7908</v>
@@ -4192,7 +4203,7 @@
         <v>23.495</v>
       </c>
       <c r="E66" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F66" s="11" t="n">
         <v>90</v>
@@ -4200,10 +4211,10 @@
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="9" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C67" s="11" t="n">
         <v>22.733</v>
@@ -4212,7 +4223,7 @@
         <v>13.8176</v>
       </c>
       <c r="E67" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F67" s="11" t="n">
         <v>90</v>
@@ -4220,10 +4231,10 @@
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="9" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C68" s="11" t="n">
         <v>46.047</v>
@@ -4232,7 +4243,7 @@
         <v>10.3981</v>
       </c>
       <c r="E68" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F68" s="11" t="n">
         <v>90</v>
@@ -4240,10 +4251,10 @@
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="9" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C69" s="11" t="n">
         <v>69.8595</v>
@@ -4252,7 +4263,7 @@
         <v>10.3981</v>
       </c>
       <c r="E69" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F69" s="11" t="n">
         <v>90</v>
@@ -4260,10 +4271,10 @@
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="9" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C70" s="11" t="n">
         <v>110.3408</v>
@@ -4272,7 +4283,7 @@
         <v>10.3981</v>
       </c>
       <c r="E70" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F70" s="11" t="n">
         <v>90</v>
@@ -4280,10 +4291,10 @@
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C71" s="11" t="n">
         <v>150.822</v>
@@ -4292,7 +4303,7 @@
         <v>9.2075</v>
       </c>
       <c r="E71" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F71" s="11" t="n">
         <v>90</v>
@@ -4300,10 +4311,10 @@
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="9" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C72" s="11" t="n">
         <v>155.5845</v>
@@ -4312,7 +4323,7 @@
         <v>9.2075</v>
       </c>
       <c r="E72" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F72" s="11" t="n">
         <v>90</v>
@@ -4320,10 +4331,10 @@
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="9" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C73" s="11" t="n">
         <v>207.972</v>
@@ -4332,7 +4343,7 @@
         <v>15.1606</v>
       </c>
       <c r="E73" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F73" s="11" t="n">
         <v>90</v>
@@ -4340,10 +4351,10 @@
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="9" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C74" s="11" t="n">
         <v>211.5439</v>
@@ -4352,7 +4363,7 @@
         <v>15.1606</v>
       </c>
       <c r="E74" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F74" s="11" t="n">
         <v>90</v>
@@ -4360,10 +4371,10 @@
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="9" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C75" s="11" t="n">
         <v>243.6908</v>
@@ -4372,7 +4383,7 @@
         <v>16.3513</v>
       </c>
       <c r="E75" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F75" s="11" t="n">
         <v>90</v>
@@ -4380,10 +4391,10 @@
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C76" s="11" t="n">
         <v>262.7408</v>
@@ -4392,7 +4403,7 @@
         <v>13.97</v>
       </c>
       <c r="E76" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F76" s="11" t="n">
         <v>90</v>
@@ -4400,10 +4411,10 @@
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C77" s="11" t="n">
         <v>281.7908</v>
@@ -4412,7 +4423,7 @@
         <v>13.97</v>
       </c>
       <c r="E77" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F77" s="11" t="n">
         <v>90</v>
@@ -4420,10 +4431,10 @@
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="9" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C78" s="11" t="n">
         <v>18.1814</v>
@@ -4432,7 +4443,7 @@
         <v>83.07</v>
       </c>
       <c r="E78" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F78" s="11" t="n">
         <v>270</v>
@@ -4443,7 +4454,7 @@
         <v>73</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C79" s="11" t="n">
         <v>14.2314</v>
@@ -4452,7 +4463,7 @@
         <v>82.27</v>
       </c>
       <c r="E79" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F79" s="11" t="n">
         <v>90</v>
@@ -4472,7 +4483,7 @@
         <v>37.084</v>
       </c>
       <c r="E80" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F80" s="11" t="n">
         <v>270</v>
@@ -4480,10 +4491,10 @@
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="9" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C81" s="11" t="n">
         <v>4.3751</v>
@@ -4492,7 +4503,7 @@
         <v>79.4544</v>
       </c>
       <c r="E81" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F81" s="11" t="n">
         <v>90</v>
@@ -4500,10 +4511,10 @@
     </row>
     <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="9" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C82" s="11" t="n">
         <v>23.4251</v>
@@ -4512,7 +4523,7 @@
         <v>79.4544</v>
       </c>
       <c r="E82" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F82" s="11" t="n">
         <v>90</v>
@@ -4520,10 +4531,10 @@
     </row>
     <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="9" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C83" s="11" t="n">
         <v>42.4751</v>
@@ -4532,7 +4543,7 @@
         <v>79.4544</v>
       </c>
       <c r="E83" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F83" s="11" t="n">
         <v>90</v>
@@ -4540,10 +4551,10 @@
     </row>
     <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="9" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C84" s="11" t="n">
         <v>61.5251</v>
@@ -4552,7 +4563,7 @@
         <v>79.4544</v>
       </c>
       <c r="E84" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F84" s="11" t="n">
         <v>90</v>
@@ -4560,10 +4571,10 @@
     </row>
     <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C85" s="11" t="n">
         <v>80.5751</v>
@@ -4572,7 +4583,7 @@
         <v>79.4544</v>
       </c>
       <c r="E85" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F85" s="11" t="n">
         <v>90</v>
@@ -4580,10 +4591,10 @@
     </row>
     <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="9" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C86" s="11" t="n">
         <v>99.6251</v>
@@ -4592,7 +4603,7 @@
         <v>79.4544</v>
       </c>
       <c r="E86" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F86" s="11" t="n">
         <v>90</v>
@@ -4600,10 +4611,10 @@
     </row>
     <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="9" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C87" s="11" t="n">
         <v>118.6751</v>
@@ -4612,7 +4623,7 @@
         <v>79.4544</v>
       </c>
       <c r="E87" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F87" s="11" t="n">
         <v>90</v>
@@ -4620,10 +4631,10 @@
     </row>
     <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="9" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C88" s="11" t="n">
         <v>137.7251</v>
@@ -4632,7 +4643,7 @@
         <v>79.4544</v>
       </c>
       <c r="E88" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F88" s="11" t="n">
         <v>90</v>
@@ -4640,10 +4651,10 @@
     </row>
     <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="9" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C89" s="11" t="n">
         <v>156.7751</v>
@@ -4652,7 +4663,7 @@
         <v>79.4544</v>
       </c>
       <c r="E89" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F89" s="11" t="n">
         <v>90</v>
@@ -4660,10 +4671,10 @@
     </row>
     <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="9" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C90" s="11" t="n">
         <v>175.8251</v>
@@ -4672,7 +4683,7 @@
         <v>79.4544</v>
       </c>
       <c r="E90" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F90" s="11" t="n">
         <v>90</v>
@@ -4680,10 +4691,10 @@
     </row>
     <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="9" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C91" s="11" t="n">
         <v>194.8751</v>
@@ -4692,7 +4703,7 @@
         <v>79.4544</v>
       </c>
       <c r="E91" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F91" s="11" t="n">
         <v>90</v>
@@ -4700,10 +4711,10 @@
     </row>
     <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="9" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C92" s="11" t="n">
         <v>213.9252</v>
@@ -4712,7 +4723,7 @@
         <v>79.4544</v>
       </c>
       <c r="E92" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F92" s="11" t="n">
         <v>90</v>
@@ -4720,10 +4731,10 @@
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="9" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C93" s="11" t="n">
         <v>232.9751</v>
@@ -4732,7 +4743,7 @@
         <v>79.4544</v>
       </c>
       <c r="E93" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F93" s="11" t="n">
         <v>90</v>
@@ -4740,10 +4751,10 @@
     </row>
     <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C94" s="11" t="n">
         <v>250.8345</v>
@@ -4752,7 +4763,7 @@
         <v>79.4544</v>
       </c>
       <c r="E94" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F94" s="11" t="n">
         <v>90</v>
@@ -4760,10 +4771,10 @@
     </row>
     <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="9" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C95" s="11" t="n">
         <v>271.0752</v>
@@ -4772,7 +4783,7 @@
         <v>79.4544</v>
       </c>
       <c r="E95" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F95" s="11" t="n">
         <v>90</v>
@@ -4780,10 +4791,10 @@
     </row>
     <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="9" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C96" s="11" t="n">
         <v>9.1376</v>
@@ -4792,7 +4803,7 @@
         <v>60.4044</v>
       </c>
       <c r="E96" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F96" s="11" t="n">
         <v>90</v>
@@ -4800,10 +4811,10 @@
     </row>
     <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="9" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C97" s="11" t="n">
         <v>32.9502</v>
@@ -4812,7 +4823,7 @@
         <v>62.7856</v>
       </c>
       <c r="E97" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F97" s="11" t="n">
         <v>90</v>
@@ -4820,10 +4831,10 @@
     </row>
     <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="9" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C98" s="11" t="n">
         <v>52.07</v>
@@ -4832,7 +4843,7 @@
         <v>61.3798</v>
       </c>
       <c r="E98" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F98" s="11" t="n">
         <v>90</v>
@@ -4840,10 +4851,10 @@
     </row>
     <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="9" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C99" s="11" t="n">
         <v>71.0502</v>
@@ -4852,7 +4863,7 @@
         <v>60.4044</v>
       </c>
       <c r="E99" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F99" s="11" t="n">
         <v>90</v>
@@ -4860,10 +4871,10 @@
     </row>
     <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="9" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C100" s="11" t="n">
         <v>90.1001</v>
@@ -4872,7 +4883,7 @@
         <v>60.4044</v>
       </c>
       <c r="E100" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F100" s="11" t="n">
         <v>90</v>
@@ -4880,10 +4891,10 @@
     </row>
     <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="9" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C101" s="11" t="n">
         <v>109.1501</v>
@@ -4892,7 +4903,7 @@
         <v>60.4044</v>
       </c>
       <c r="E101" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F101" s="11" t="n">
         <v>90</v>
@@ -4900,10 +4911,10 @@
     </row>
     <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="9" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C102" s="11" t="n">
         <v>128.2002</v>
@@ -4912,7 +4923,7 @@
         <v>60.4044</v>
       </c>
       <c r="E102" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F102" s="11" t="n">
         <v>90</v>
@@ -4920,10 +4931,10 @@
     </row>
     <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="9" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C103" s="11" t="n">
         <v>147.2501</v>
@@ -4932,7 +4943,7 @@
         <v>60.4044</v>
       </c>
       <c r="E103" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F103" s="11" t="n">
         <v>90</v>
@@ -4940,10 +4951,10 @@
     </row>
     <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="9" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C104" s="11" t="n">
         <v>166.3002</v>
@@ -4952,7 +4963,7 @@
         <v>60.4044</v>
       </c>
       <c r="E104" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F104" s="11" t="n">
         <v>90</v>
@@ -4960,10 +4971,10 @@
     </row>
     <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="9" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C105" s="11" t="n">
         <v>185.3501</v>
@@ -4972,7 +4983,7 @@
         <v>60.4044</v>
       </c>
       <c r="E105" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F105" s="11" t="n">
         <v>90</v>
@@ -4980,10 +4991,10 @@
     </row>
     <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="9" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C106" s="11" t="n">
         <v>204.4001</v>
@@ -4992,7 +5003,7 @@
         <v>60.4044</v>
       </c>
       <c r="E106" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F106" s="11" t="n">
         <v>90</v>
@@ -5000,10 +5011,10 @@
     </row>
     <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="9" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C107" s="11" t="n">
         <v>223.4501</v>
@@ -5012,7 +5023,7 @@
         <v>60.4044</v>
       </c>
       <c r="E107" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F107" s="11" t="n">
         <v>90</v>
@@ -5020,10 +5031,10 @@
     </row>
     <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="9" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C108" s="11" t="n">
         <v>242.5001</v>
@@ -5032,7 +5043,7 @@
         <v>60.4044</v>
       </c>
       <c r="E108" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F108" s="11" t="n">
         <v>90</v>
@@ -5040,10 +5051,10 @@
     </row>
     <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="9" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C109" s="11" t="n">
         <v>266.3126</v>
@@ -5052,7 +5063,7 @@
         <v>60.4044</v>
       </c>
       <c r="E109" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F109" s="11" t="n">
         <v>90</v>
@@ -5060,10 +5071,10 @@
     </row>
     <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="9" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C110" s="11" t="n">
         <v>7.947</v>
@@ -5072,7 +5083,7 @@
         <v>43.7356</v>
       </c>
       <c r="E110" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F110" s="11" t="n">
         <v>90</v>
@@ -5080,10 +5091,10 @@
     </row>
     <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="9" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C111" s="11" t="n">
         <v>37.7126</v>
@@ -5092,7 +5103,7 @@
         <v>41.3544</v>
       </c>
       <c r="E111" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F111" s="11" t="n">
         <v>90</v>
@@ -5100,10 +5111,10 @@
     </row>
     <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="9" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C112" s="11" t="n">
         <v>56.7627</v>
@@ -5112,7 +5123,7 @@
         <v>41.3544</v>
       </c>
       <c r="E112" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F112" s="11" t="n">
         <v>90</v>
@@ -5120,10 +5131,10 @@
     </row>
     <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="9" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C113" s="11" t="n">
         <v>75.8126</v>
@@ -5132,7 +5143,7 @@
         <v>41.3544</v>
       </c>
       <c r="E113" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F113" s="11" t="n">
         <v>90</v>
@@ -5140,10 +5151,10 @@
     </row>
     <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="9" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C114" s="11" t="n">
         <v>94.8627</v>
@@ -5152,7 +5163,7 @@
         <v>41.3544</v>
       </c>
       <c r="E114" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F114" s="11" t="n">
         <v>90</v>
@@ -5160,10 +5171,10 @@
     </row>
     <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="9" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C115" s="11" t="n">
         <v>113.9126</v>
@@ -5172,7 +5183,7 @@
         <v>41.3544</v>
       </c>
       <c r="E115" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F115" s="11" t="n">
         <v>90</v>
@@ -5180,10 +5191,10 @@
     </row>
     <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="9" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C116" s="11" t="n">
         <v>132.9626</v>
@@ -5192,7 +5203,7 @@
         <v>41.3544</v>
       </c>
       <c r="E116" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F116" s="11" t="n">
         <v>90</v>
@@ -5200,10 +5211,10 @@
     </row>
     <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="9" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C117" s="11" t="n">
         <v>152.0126</v>
@@ -5212,7 +5223,7 @@
         <v>41.3544</v>
       </c>
       <c r="E117" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F117" s="11" t="n">
         <v>90</v>
@@ -5220,10 +5231,10 @@
     </row>
     <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="9" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C118" s="11" t="n">
         <v>171.0626</v>
@@ -5232,7 +5243,7 @@
         <v>41.3544</v>
       </c>
       <c r="E118" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F118" s="11" t="n">
         <v>90</v>
@@ -5240,10 +5251,10 @@
     </row>
     <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="9" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C119" s="11" t="n">
         <v>190.1127</v>
@@ -5252,7 +5263,7 @@
         <v>41.3544</v>
       </c>
       <c r="E119" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F119" s="11" t="n">
         <v>90</v>
@@ -5260,10 +5271,10 @@
     </row>
     <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="9" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C120" s="11" t="n">
         <v>209.1626</v>
@@ -5272,7 +5283,7 @@
         <v>41.3544</v>
       </c>
       <c r="E120" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F120" s="11" t="n">
         <v>90</v>
@@ -5280,10 +5291,10 @@
     </row>
     <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="9" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C121" s="11" t="n">
         <v>228.2126</v>
@@ -5292,7 +5303,7 @@
         <v>41.3544</v>
       </c>
       <c r="E121" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F121" s="11" t="n">
         <v>90</v>
@@ -5300,10 +5311,10 @@
     </row>
     <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="9" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C122" s="11" t="n">
         <v>247.2626</v>
@@ -5312,7 +5323,7 @@
         <v>41.3544</v>
       </c>
       <c r="E122" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F122" s="11" t="n">
         <v>90</v>
@@ -5320,10 +5331,10 @@
     </row>
     <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="9" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C123" s="11" t="n">
         <v>259.1689</v>
@@ -5332,7 +5343,7 @@
         <v>41.3544</v>
       </c>
       <c r="E123" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F123" s="11" t="n">
         <v>90</v>
@@ -5340,10 +5351,10 @@
     </row>
     <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="9" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C124" s="11" t="n">
         <v>6.7564</v>
@@ -5352,7 +5363,7 @@
         <v>24.6856</v>
       </c>
       <c r="E124" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F124" s="11" t="n">
         <v>90</v>
@@ -5360,10 +5371,10 @@
     </row>
     <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="9" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C125" s="11" t="n">
         <v>28.1876</v>
@@ -5372,7 +5383,7 @@
         <v>22.3044</v>
       </c>
       <c r="E125" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F125" s="11" t="n">
         <v>90</v>
@@ -5380,10 +5391,10 @@
     </row>
     <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="9" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C126" s="11" t="n">
         <v>47.2376</v>
@@ -5392,7 +5403,7 @@
         <v>22.3044</v>
       </c>
       <c r="E126" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F126" s="11" t="n">
         <v>90</v>
@@ -5400,10 +5411,10 @@
     </row>
     <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="9" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C127" s="11" t="n">
         <v>66.2876</v>
@@ -5412,7 +5423,7 @@
         <v>22.3044</v>
       </c>
       <c r="E127" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F127" s="11" t="n">
         <v>90</v>
@@ -5420,10 +5431,10 @@
     </row>
     <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="9" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C128" s="11" t="n">
         <v>85.3376</v>
@@ -5432,7 +5443,7 @@
         <v>22.3044</v>
       </c>
       <c r="E128" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F128" s="11" t="n">
         <v>90</v>
@@ -5440,10 +5451,10 @@
     </row>
     <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="9" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C129" s="11" t="n">
         <v>104.3876</v>
@@ -5452,7 +5463,7 @@
         <v>22.3044</v>
       </c>
       <c r="E129" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F129" s="11" t="n">
         <v>90</v>
@@ -5460,10 +5471,10 @@
     </row>
     <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="9" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C130" s="11" t="n">
         <v>123.4376</v>
@@ -5472,7 +5483,7 @@
         <v>22.3044</v>
       </c>
       <c r="E130" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F130" s="11" t="n">
         <v>90</v>
@@ -5480,10 +5491,10 @@
     </row>
     <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="9" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C131" s="11" t="n">
         <v>142.4877</v>
@@ -5492,7 +5503,7 @@
         <v>22.3044</v>
       </c>
       <c r="E131" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F131" s="11" t="n">
         <v>90</v>
@@ -5500,10 +5511,10 @@
     </row>
     <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="9" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C132" s="11" t="n">
         <v>161.5376</v>
@@ -5512,7 +5523,7 @@
         <v>22.3044</v>
       </c>
       <c r="E132" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F132" s="11" t="n">
         <v>90</v>
@@ -5520,10 +5531,10 @@
     </row>
     <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="9" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C133" s="11" t="n">
         <v>180.5876</v>
@@ -5532,7 +5543,7 @@
         <v>22.3044</v>
       </c>
       <c r="E133" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F133" s="11" t="n">
         <v>90</v>
@@ -5540,10 +5551,10 @@
     </row>
     <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="9" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C134" s="11" t="n">
         <v>199.6376</v>
@@ -5552,7 +5563,7 @@
         <v>22.3044</v>
       </c>
       <c r="E134" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F134" s="11" t="n">
         <v>90</v>
@@ -5560,10 +5571,10 @@
     </row>
     <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="9" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C135" s="11" t="n">
         <v>218.6876</v>
@@ -5572,7 +5583,7 @@
         <v>22.3044</v>
       </c>
       <c r="E135" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F135" s="11" t="n">
         <v>90</v>
@@ -5580,10 +5591,10 @@
     </row>
     <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="9" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C136" s="11" t="n">
         <v>254.4064</v>
@@ -5592,7 +5603,7 @@
         <v>22.3044</v>
       </c>
       <c r="E136" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F136" s="11" t="n">
         <v>90</v>
@@ -5600,10 +5611,10 @@
     </row>
     <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="9" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C137" s="11" t="n">
         <v>275.8376</v>
@@ -5612,7 +5623,7 @@
         <v>19.9231</v>
       </c>
       <c r="E137" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F137" s="11" t="n">
         <v>0</v>
@@ -5620,10 +5631,10 @@
     </row>
     <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="9" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C138" s="11" t="n">
         <v>6.7564</v>
@@ -5632,7 +5643,7 @@
         <v>3.2544</v>
       </c>
       <c r="E138" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F138" s="11" t="n">
         <v>90</v>
@@ -5640,10 +5651,10 @@
     </row>
     <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="9" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C139" s="11" t="n">
         <v>30.5689</v>
@@ -5652,7 +5663,7 @@
         <v>3.2544</v>
       </c>
       <c r="E139" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F139" s="11" t="n">
         <v>90</v>
@@ -5660,10 +5671,10 @@
     </row>
     <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="9" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C140" s="11" t="n">
         <v>54.3814</v>
@@ -5672,7 +5683,7 @@
         <v>3.2544</v>
       </c>
       <c r="E140" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F140" s="11" t="n">
         <v>90</v>
@@ -5680,10 +5691,10 @@
     </row>
     <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="9" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C141" s="11" t="n">
         <v>117.6782</v>
@@ -5692,7 +5703,7 @@
         <v>3.2258</v>
       </c>
       <c r="E141" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F141" s="11" t="n">
         <v>90</v>
@@ -5700,10 +5711,10 @@
     </row>
     <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C142" s="11" t="n">
         <v>121.0564</v>
@@ -5712,7 +5723,7 @@
         <v>3.2544</v>
       </c>
       <c r="E142" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F142" s="11" t="n">
         <v>90</v>
@@ -5720,10 +5731,10 @@
     </row>
     <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C143" s="11" t="n">
         <v>159.1564</v>
@@ -5732,7 +5743,7 @@
         <v>4.445</v>
       </c>
       <c r="E143" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F143" s="11" t="n">
         <v>90</v>
@@ -5740,10 +5751,10 @@
     </row>
     <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C144" s="11" t="n">
         <v>206.7814</v>
@@ -5752,7 +5763,7 @@
         <v>3.2544</v>
       </c>
       <c r="E144" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F144" s="11" t="n">
         <v>90</v>
@@ -5760,10 +5771,10 @@
     </row>
     <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="9" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C145" s="11" t="n">
         <v>230.5939</v>
@@ -5772,7 +5783,7 @@
         <v>3.2544</v>
       </c>
       <c r="E145" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F145" s="11" t="n">
         <v>90</v>
@@ -5780,10 +5791,10 @@
     </row>
     <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="9" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C146" s="11" t="n">
         <v>234.1658</v>
@@ -5792,7 +5803,7 @@
         <v>3.2544</v>
       </c>
       <c r="E146" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F146" s="11" t="n">
         <v>90</v>
@@ -5800,10 +5811,10 @@
     </row>
     <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B147" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C147" s="11" t="n">
         <v>253.1364</v>
@@ -5812,7 +5823,7 @@
         <v>2.413</v>
       </c>
       <c r="E147" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F147" s="11" t="n">
         <v>270</v>
@@ -5820,10 +5831,10 @@
     </row>
     <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C148" s="11" t="n">
         <v>267.7414</v>
@@ -5832,7 +5843,7 @@
         <v>2.032</v>
       </c>
       <c r="E148" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F148" s="11" t="n">
         <v>90</v>
@@ -5840,10 +5851,10 @@
     </row>
     <row r="149" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C149" s="11" t="n">
         <v>29.2354</v>
@@ -5852,7 +5863,7 @@
         <v>43.18</v>
       </c>
       <c r="E149" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F149" s="11" t="n">
         <v>0</v>
@@ -5860,10 +5871,10 @@
     </row>
     <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C150" s="11" t="n">
         <v>24.6158</v>
@@ -5872,7 +5883,7 @@
         <v>43.7356</v>
       </c>
       <c r="E150" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F150" s="11" t="n">
         <v>180</v>
@@ -5880,10 +5891,10 @@
     </row>
     <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B151" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C151" s="11" t="n">
         <v>39.3954</v>
@@ -5892,7 +5903,7 @@
         <v>58.166</v>
       </c>
       <c r="E151" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F151" s="11" t="n">
         <v>180</v>
@@ -5900,10 +5911,10 @@
     </row>
     <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="9" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C152" s="11" t="n">
         <v>19.2814</v>
@@ -5912,7 +5923,7 @@
         <v>78.82</v>
       </c>
       <c r="E152" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F152" s="11" t="n">
         <v>90</v>
@@ -5920,10 +5931,10 @@
     </row>
     <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="9" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C153" s="11" t="n">
         <v>17.1314</v>
@@ -5932,7 +5943,7 @@
         <v>78.82</v>
       </c>
       <c r="E153" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F153" s="11" t="n">
         <v>90</v>
@@ -5940,10 +5951,10 @@
     </row>
     <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="9" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B154" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C154" s="11" t="n">
         <v>12.065</v>
@@ -5952,7 +5963,7 @@
         <v>87.4268</v>
       </c>
       <c r="E154" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F154" s="11" t="n">
         <v>270</v>
@@ -5960,10 +5971,10 @@
     </row>
     <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="9" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B155" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C155" s="11" t="n">
         <v>26.0314</v>
@@ -5972,7 +5983,7 @@
         <v>91.07</v>
       </c>
       <c r="E155" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F155" s="11" t="n">
         <v>180</v>
@@ -5980,10 +5991,10 @@
     </row>
     <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C156" s="11" t="n">
         <v>28.0924</v>
@@ -5992,7 +6003,7 @@
         <v>36.576</v>
       </c>
       <c r="E156" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F156" s="11" t="n">
         <v>270</v>
@@ -6000,10 +6011,10 @@
     </row>
     <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B157" s="9" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C157" s="11" t="n">
         <v>29.3783</v>
@@ -6012,7 +6023,7 @@
         <v>53.2606</v>
       </c>
       <c r="E157" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F157" s="11" t="n">
         <v>270</v>
@@ -6020,10 +6031,10 @@
     </row>
     <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B158" s="9" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C158" s="11" t="n">
         <v>18.1922</v>
@@ -6032,7 +6043,7 @@
         <v>87.6436</v>
       </c>
       <c r="E158" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F158" s="11" t="n">
         <v>0</v>
@@ -6040,10 +6051,10 @@
     </row>
     <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B159" s="9" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C159" s="11" t="n">
         <v>45.5168</v>
@@ -6052,7 +6063,7 @@
         <v>59.2582</v>
       </c>
       <c r="E159" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F159" s="11" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Update: files for production
</commit_message>
<xml_diff>
--- a/fabrication/elecrow/CO60-PCBA-Quotation.xlsx
+++ b/fabrication/elecrow/CO60-PCBA-Quotation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PCB Specification" sheetId="1" state="visible" r:id="rId2"/>
@@ -1186,7 +1186,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1240,6 +1240,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="SimSun"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1277,12 +1284,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -1333,7 +1346,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1394,6 +1407,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1402,15 +1419,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1437,13 +1454,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>559080</xdr:colOff>
+      <xdr:colOff>558720</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>24840</xdr:rowOff>
+      <xdr:rowOff>24480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Image 1" descr="Picture generated by PCBNEW "/>
+        <xdr:cNvPr id="0" name="Image 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1453,7 +1470,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10426680" cy="3701160"/>
+          <a:ext cx="10426320" cy="3700800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1481,8 +1498,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="7.92712550607287"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="26" min="6" style="0" width="7.92712550607287"/>
@@ -1659,8 +1676,8 @@
   </sheetPr>
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N17" activeCellId="0" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1668,14 +1685,14 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.82186234817814"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.92712550607287"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.8137651821862"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="10" min="9" style="0" width="7.92712550607287"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.0323886639676"/>
     <col collapsed="false" hidden="false" max="26" min="15" style="0" width="7.92712550607287"/>
     <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.57085020242915"/>
   </cols>
@@ -2750,7 +2767,7 @@
       <c r="E22" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="16" t="s">
         <v>152</v>
       </c>
       <c r="G22" s="13" t="s">
@@ -2785,27 +2802,27 @@
       <c r="Z22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="17" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="H23" s="17" t="n">
+      <c r="H23" s="18" t="n">
         <f aca="false">SUM(H3:H22)</f>
         <v>489</v>
       </c>
-      <c r="I23" s="17" t="n">
+      <c r="I23" s="18" t="n">
         <f aca="false">SUM(I2:I20)</f>
         <v>0</v>
       </c>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
@@ -2821,19 +2838,19 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="16"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
@@ -2849,21 +2866,21 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16"/>
-      <c r="B25" s="19" t="s">
+      <c r="A25" s="17"/>
+      <c r="B25" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
@@ -2879,21 +2896,21 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="16"/>
-      <c r="B26" s="19" t="s">
+      <c r="A26" s="17"/>
+      <c r="B26" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
@@ -2943,7 +2960,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2966,38 +2983,38 @@
   </sheetPr>
   <dimension ref="A1:F194"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="26" min="6" style="0" width="7.92712550607287"/>
     <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="17" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3014,7 +3031,7 @@
       <c r="D2" s="0" t="n">
         <v>62.35</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F2" s="0" t="n">
@@ -3034,7 +3051,7 @@
       <c r="D3" s="0" t="n">
         <v>55.82</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F3" s="0" t="n">
@@ -3054,7 +3071,7 @@
       <c r="D4" s="0" t="n">
         <v>60.41</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F4" s="0" t="n">
@@ -3074,7 +3091,7 @@
       <c r="D5" s="0" t="n">
         <v>55.75</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F5" s="0" t="n">
@@ -3094,7 +3111,7 @@
       <c r="D6" s="0" t="n">
         <v>55.75</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F6" s="0" t="n">
@@ -3114,7 +3131,7 @@
       <c r="D7" s="0" t="n">
         <v>53.29428</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F7" s="0" t="n">
@@ -3134,7 +3151,7 @@
       <c r="D8" s="0" t="n">
         <v>53.286</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F8" s="0" t="n">
@@ -3154,7 +3171,7 @@
       <c r="D9" s="0" t="n">
         <v>46.9894</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F9" s="0" t="n">
@@ -3174,7 +3191,7 @@
       <c r="D10" s="0" t="n">
         <v>50.62</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F10" s="0" t="n">
@@ -3194,7 +3211,7 @@
       <c r="D11" s="0" t="n">
         <v>63.92</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F11" s="0" t="n">
@@ -3214,7 +3231,7 @@
       <c r="D12" s="0" t="n">
         <v>58.3946</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F12" s="0" t="n">
@@ -3234,7 +3251,7 @@
       <c r="D13" s="0" t="n">
         <v>76.18</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F13" s="0" t="n">
@@ -3254,7 +3271,7 @@
       <c r="D14" s="0" t="n">
         <v>75.59</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F14" s="0" t="n">
@@ -3274,7 +3291,7 @@
       <c r="D15" s="0" t="n">
         <v>75.66</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F15" s="0" t="n">
@@ -3294,7 +3311,7 @@
       <c r="D16" s="0" t="n">
         <v>76.47</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F16" s="0" t="n">
@@ -3314,7 +3331,7 @@
       <c r="D17" s="0" t="n">
         <v>75.68</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F17" s="0" t="n">
@@ -3334,7 +3351,7 @@
       <c r="D18" s="0" t="n">
         <v>76.03</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F18" s="0" t="n">
@@ -3354,7 +3371,7 @@
       <c r="D19" s="0" t="n">
         <v>75.92</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F19" s="0" t="n">
@@ -3374,7 +3391,7 @@
       <c r="D20" s="0" t="n">
         <v>75.76</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F20" s="0" t="n">
@@ -3394,7 +3411,7 @@
       <c r="D21" s="0" t="n">
         <v>18.89</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F21" s="0" t="n">
@@ -3414,7 +3431,7 @@
       <c r="D22" s="0" t="n">
         <v>20.07</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F22" s="0" t="n">
@@ -3434,7 +3451,7 @@
       <c r="D23" s="0" t="n">
         <v>22.81</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F23" s="0" t="n">
@@ -3454,7 +3471,7 @@
       <c r="D24" s="0" t="n">
         <v>20.76</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F24" s="0" t="n">
@@ -3474,7 +3491,7 @@
       <c r="D25" s="0" t="n">
         <v>18.44</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F25" s="0" t="n">
@@ -3494,7 +3511,7 @@
       <c r="D26" s="0" t="n">
         <v>23.07</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F26" s="0" t="n">
@@ -3514,7 +3531,7 @@
       <c r="D27" s="0" t="n">
         <v>18.48</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F27" s="0" t="n">
@@ -3534,7 +3551,7 @@
       <c r="D28" s="0" t="n">
         <v>18.95</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F28" s="0" t="n">
@@ -3554,7 +3571,7 @@
       <c r="D29" s="0" t="n">
         <v>91.44</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F29" s="0" t="n">
@@ -3574,7 +3591,7 @@
       <c r="D30" s="0" t="n">
         <v>86.598125</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F30" s="0" t="n">
@@ -3594,7 +3611,7 @@
       <c r="D31" s="0" t="n">
         <v>86.598125</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F31" s="0" t="n">
@@ -3614,7 +3631,7 @@
       <c r="D32" s="0" t="n">
         <v>88.93</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="E32" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F32" s="0" t="n">
@@ -3634,7 +3651,7 @@
       <c r="D33" s="0" t="n">
         <v>86.598125</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F33" s="0" t="n">
@@ -3654,7 +3671,7 @@
       <c r="D34" s="0" t="n">
         <v>86.598125</v>
       </c>
-      <c r="E34" s="16" t="s">
+      <c r="E34" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F34" s="0" t="n">
@@ -3674,7 +3691,7 @@
       <c r="D35" s="0" t="n">
         <v>86.598125</v>
       </c>
-      <c r="E35" s="16" t="s">
+      <c r="E35" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F35" s="0" t="n">
@@ -3694,7 +3711,7 @@
       <c r="D36" s="0" t="n">
         <v>86.598125</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="E36" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F36" s="0" t="n">
@@ -3714,7 +3731,7 @@
       <c r="D37" s="0" t="n">
         <v>86.598125</v>
       </c>
-      <c r="E37" s="16" t="s">
+      <c r="E37" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F37" s="0" t="n">
@@ -3734,7 +3751,7 @@
       <c r="D38" s="0" t="n">
         <v>88.85</v>
       </c>
-      <c r="E38" s="16" t="s">
+      <c r="E38" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F38" s="0" t="n">
@@ -3754,7 +3771,7 @@
       <c r="D39" s="0" t="n">
         <v>86.598125</v>
       </c>
-      <c r="E39" s="16" t="s">
+      <c r="E39" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F39" s="0" t="n">
@@ -3774,7 +3791,7 @@
       <c r="D40" s="0" t="n">
         <v>86.598125</v>
       </c>
-      <c r="E40" s="16" t="s">
+      <c r="E40" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F40" s="0" t="n">
@@ -3794,7 +3811,7 @@
       <c r="D41" s="0" t="n">
         <v>86.598125</v>
       </c>
-      <c r="E41" s="16" t="s">
+      <c r="E41" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F41" s="0" t="n">
@@ -3814,7 +3831,7 @@
       <c r="D42" s="0" t="n">
         <v>90.17</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="E42" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F42" s="0" t="n">
@@ -3834,7 +3851,7 @@
       <c r="D43" s="0" t="n">
         <v>90.17</v>
       </c>
-      <c r="E43" s="16" t="s">
+      <c r="E43" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F43" s="0" t="n">
@@ -3854,7 +3871,7 @@
       <c r="D44" s="0" t="n">
         <v>71.12</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E44" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F44" s="0" t="n">
@@ -3874,7 +3891,7 @@
       <c r="D45" s="0" t="n">
         <v>69.42</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="E45" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F45" s="0" t="n">
@@ -3894,7 +3911,7 @@
       <c r="D46" s="0" t="n">
         <v>67.548125</v>
       </c>
-      <c r="E46" s="16" t="s">
+      <c r="E46" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F46" s="0" t="n">
@@ -3914,7 +3931,7 @@
       <c r="D47" s="0" t="n">
         <v>67.548125</v>
       </c>
-      <c r="E47" s="16" t="s">
+      <c r="E47" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F47" s="0" t="n">
@@ -3934,7 +3951,7 @@
       <c r="D48" s="0" t="n">
         <v>67.548125</v>
       </c>
-      <c r="E48" s="16" t="s">
+      <c r="E48" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F48" s="0" t="n">
@@ -3954,7 +3971,7 @@
       <c r="D49" s="0" t="n">
         <v>67.548125</v>
       </c>
-      <c r="E49" s="16" t="s">
+      <c r="E49" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F49" s="0" t="n">
@@ -3974,7 +3991,7 @@
       <c r="D50" s="0" t="n">
         <v>67.548125</v>
       </c>
-      <c r="E50" s="16" t="s">
+      <c r="E50" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F50" s="0" t="n">
@@ -3994,7 +4011,7 @@
       <c r="D51" s="0" t="n">
         <v>67.548125</v>
       </c>
-      <c r="E51" s="16" t="s">
+      <c r="E51" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F51" s="0" t="n">
@@ -4014,7 +4031,7 @@
       <c r="D52" s="0" t="n">
         <v>67.548125</v>
       </c>
-      <c r="E52" s="16" t="s">
+      <c r="E52" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F52" s="0" t="n">
@@ -4034,7 +4051,7 @@
       <c r="D53" s="0" t="n">
         <v>67.548125</v>
       </c>
-      <c r="E53" s="16" t="s">
+      <c r="E53" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F53" s="0" t="n">
@@ -4054,7 +4071,7 @@
       <c r="D54" s="0" t="n">
         <v>67.548125</v>
       </c>
-      <c r="E54" s="16" t="s">
+      <c r="E54" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F54" s="0" t="n">
@@ -4074,7 +4091,7 @@
       <c r="D55" s="0" t="n">
         <v>67.548125</v>
       </c>
-      <c r="E55" s="16" t="s">
+      <c r="E55" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F55" s="0" t="n">
@@ -4094,7 +4111,7 @@
       <c r="D56" s="0" t="n">
         <v>69.929375</v>
       </c>
-      <c r="E56" s="16" t="s">
+      <c r="E56" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F56" s="0" t="n">
@@ -4114,7 +4131,7 @@
       <c r="D57" s="0" t="n">
         <v>71.12</v>
       </c>
-      <c r="E57" s="16" t="s">
+      <c r="E57" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F57" s="0" t="n">
@@ -4134,7 +4151,7 @@
       <c r="D58" s="0" t="n">
         <v>42.545</v>
       </c>
-      <c r="E58" s="16" t="s">
+      <c r="E58" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F58" s="0" t="n">
@@ -4154,7 +4171,7 @@
       <c r="D59" s="0" t="n">
         <v>48.498125</v>
       </c>
-      <c r="E59" s="16" t="s">
+      <c r="E59" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F59" s="0" t="n">
@@ -4174,7 +4191,7 @@
       <c r="D60" s="0" t="n">
         <v>48.498125</v>
       </c>
-      <c r="E60" s="16" t="s">
+      <c r="E60" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F60" s="0" t="n">
@@ -4194,7 +4211,7 @@
       <c r="D61" s="0" t="n">
         <v>48.498125</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="E61" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F61" s="0" t="n">
@@ -4214,7 +4231,7 @@
       <c r="D62" s="0" t="n">
         <v>48.498125</v>
       </c>
-      <c r="E62" s="16" t="s">
+      <c r="E62" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F62" s="0" t="n">
@@ -4234,7 +4251,7 @@
       <c r="D63" s="0" t="n">
         <v>48.5003</v>
       </c>
-      <c r="E63" s="16" t="s">
+      <c r="E63" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F63" s="0" t="n">
@@ -4254,7 +4271,7 @@
       <c r="D64" s="0" t="n">
         <v>48.498125</v>
       </c>
-      <c r="E64" s="16" t="s">
+      <c r="E64" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F64" s="0" t="n">
@@ -4274,7 +4291,7 @@
       <c r="D65" s="0" t="n">
         <v>48.498125</v>
       </c>
-      <c r="E65" s="16" t="s">
+      <c r="E65" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F65" s="0" t="n">
@@ -4294,7 +4311,7 @@
       <c r="D66" s="0" t="n">
         <v>48.498125</v>
       </c>
-      <c r="E66" s="16" t="s">
+      <c r="E66" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F66" s="0" t="n">
@@ -4314,7 +4331,7 @@
       <c r="D67" s="0" t="n">
         <v>48.498125</v>
       </c>
-      <c r="E67" s="16" t="s">
+      <c r="E67" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F67" s="0" t="n">
@@ -4334,7 +4351,7 @@
       <c r="D68" s="0" t="n">
         <v>48.498125</v>
       </c>
-      <c r="E68" s="16" t="s">
+      <c r="E68" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F68" s="0" t="n">
@@ -4354,7 +4371,7 @@
       <c r="D69" s="0" t="n">
         <v>48.498125</v>
       </c>
-      <c r="E69" s="16" t="s">
+      <c r="E69" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F69" s="0" t="n">
@@ -4374,7 +4391,7 @@
       <c r="D70" s="0" t="n">
         <v>54.45125</v>
       </c>
-      <c r="E70" s="16" t="s">
+      <c r="E70" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F70" s="0" t="n">
@@ -4394,7 +4411,7 @@
       <c r="D71" s="0" t="n">
         <v>47.3075</v>
       </c>
-      <c r="E71" s="16" t="s">
+      <c r="E71" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F71" s="0" t="n">
@@ -4414,7 +4431,7 @@
       <c r="D72" s="0" t="n">
         <v>29.448125</v>
       </c>
-      <c r="E72" s="16" t="s">
+      <c r="E72" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F72" s="0" t="n">
@@ -4434,7 +4451,7 @@
       <c r="D73" s="0" t="n">
         <v>29.448125</v>
       </c>
-      <c r="E73" s="16" t="s">
+      <c r="E73" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F73" s="0" t="n">
@@ -4454,7 +4471,7 @@
       <c r="D74" s="0" t="n">
         <v>29.448125</v>
       </c>
-      <c r="E74" s="16" t="s">
+      <c r="E74" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F74" s="0" t="n">
@@ -4474,7 +4491,7 @@
       <c r="D75" s="0" t="n">
         <v>29.448125</v>
       </c>
-      <c r="E75" s="16" t="s">
+      <c r="E75" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F75" s="0" t="n">
@@ -4494,7 +4511,7 @@
       <c r="D76" s="0" t="n">
         <v>29.448125</v>
       </c>
-      <c r="E76" s="16" t="s">
+      <c r="E76" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F76" s="0" t="n">
@@ -4514,7 +4531,7 @@
       <c r="D77" s="0" t="n">
         <v>29.448125</v>
       </c>
-      <c r="E77" s="16" t="s">
+      <c r="E77" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F77" s="0" t="n">
@@ -4534,7 +4551,7 @@
       <c r="D78" s="0" t="n">
         <v>29.448125</v>
       </c>
-      <c r="E78" s="16" t="s">
+      <c r="E78" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F78" s="0" t="n">
@@ -4554,7 +4571,7 @@
       <c r="D79" s="0" t="n">
         <v>29.448125</v>
       </c>
-      <c r="E79" s="16" t="s">
+      <c r="E79" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F79" s="0" t="n">
@@ -4574,7 +4591,7 @@
       <c r="D80" s="0" t="n">
         <v>29.448125</v>
       </c>
-      <c r="E80" s="16" t="s">
+      <c r="E80" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F80" s="0" t="n">
@@ -4594,7 +4611,7 @@
       <c r="D81" s="0" t="n">
         <v>29.448125</v>
       </c>
-      <c r="E81" s="16" t="s">
+      <c r="E81" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F81" s="0" t="n">
@@ -4614,7 +4631,7 @@
       <c r="D82" s="0" t="n">
         <v>29.448125</v>
       </c>
-      <c r="E82" s="16" t="s">
+      <c r="E82" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F82" s="0" t="n">
@@ -4634,7 +4651,7 @@
       <c r="D83" s="0" t="n">
         <v>29.448125</v>
       </c>
-      <c r="E83" s="16" t="s">
+      <c r="E83" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F83" s="0" t="n">
@@ -4654,7 +4671,7 @@
       <c r="D84" s="0" t="n">
         <v>29.448125</v>
       </c>
-      <c r="E84" s="16" t="s">
+      <c r="E84" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F84" s="0" t="n">
@@ -4674,7 +4691,7 @@
       <c r="D85" s="0" t="n">
         <v>23.495</v>
       </c>
-      <c r="E85" s="16" t="s">
+      <c r="E85" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F85" s="0" t="n">
@@ -4694,7 +4711,7 @@
       <c r="D86" s="0" t="n">
         <v>13.8176</v>
       </c>
-      <c r="E86" s="16" t="s">
+      <c r="E86" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F86" s="0" t="n">
@@ -4714,7 +4731,7 @@
       <c r="D87" s="0" t="n">
         <v>10.398125</v>
       </c>
-      <c r="E87" s="16" t="s">
+      <c r="E87" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F87" s="0" t="n">
@@ -4734,7 +4751,7 @@
       <c r="D88" s="0" t="n">
         <v>10.398125</v>
       </c>
-      <c r="E88" s="16" t="s">
+      <c r="E88" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F88" s="0" t="n">
@@ -4754,7 +4771,7 @@
       <c r="D89" s="0" t="n">
         <v>10.398125</v>
       </c>
-      <c r="E89" s="16" t="s">
+      <c r="E89" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F89" s="0" t="n">
@@ -4774,7 +4791,7 @@
       <c r="D90" s="0" t="n">
         <v>9.2075</v>
       </c>
-      <c r="E90" s="16" t="s">
+      <c r="E90" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F90" s="0" t="n">
@@ -4794,7 +4811,7 @@
       <c r="D91" s="0" t="n">
         <v>9.2075</v>
       </c>
-      <c r="E91" s="16" t="s">
+      <c r="E91" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F91" s="0" t="n">
@@ -4814,7 +4831,7 @@
       <c r="D92" s="0" t="n">
         <v>15.160625</v>
       </c>
-      <c r="E92" s="16" t="s">
+      <c r="E92" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F92" s="0" t="n">
@@ -4834,7 +4851,7 @@
       <c r="D93" s="0" t="n">
         <v>15.160625</v>
       </c>
-      <c r="E93" s="16" t="s">
+      <c r="E93" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F93" s="0" t="n">
@@ -4854,7 +4871,7 @@
       <c r="D94" s="0" t="n">
         <v>16.35125</v>
       </c>
-      <c r="E94" s="16" t="s">
+      <c r="E94" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F94" s="0" t="n">
@@ -4874,7 +4891,7 @@
       <c r="D95" s="0" t="n">
         <v>13.07</v>
       </c>
-      <c r="E95" s="16" t="s">
+      <c r="E95" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F95" s="0" t="n">
@@ -4894,7 +4911,7 @@
       <c r="D96" s="0" t="n">
         <v>13.97</v>
       </c>
-      <c r="E96" s="16" t="s">
+      <c r="E96" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F96" s="0" t="n">
@@ -4914,7 +4931,7 @@
       <c r="D97" s="0" t="n">
         <v>82.27</v>
       </c>
-      <c r="E97" s="16" t="s">
+      <c r="E97" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F97" s="0" t="n">
@@ -4934,7 +4951,7 @@
       <c r="D98" s="0" t="n">
         <v>37.084</v>
       </c>
-      <c r="E98" s="16" t="s">
+      <c r="E98" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F98" s="0" t="n">
@@ -4954,7 +4971,7 @@
       <c r="D99" s="0" t="n">
         <v>79.454375</v>
       </c>
-      <c r="E99" s="16" t="s">
+      <c r="E99" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F99" s="0" t="n">
@@ -4974,7 +4991,7 @@
       <c r="D100" s="0" t="n">
         <v>79.454375</v>
       </c>
-      <c r="E100" s="16" t="s">
+      <c r="E100" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F100" s="0" t="n">
@@ -4994,7 +5011,7 @@
       <c r="D101" s="0" t="n">
         <v>79.454375</v>
       </c>
-      <c r="E101" s="16" t="s">
+      <c r="E101" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F101" s="0" t="n">
@@ -5014,7 +5031,7 @@
       <c r="D102" s="0" t="n">
         <v>80.52</v>
       </c>
-      <c r="E102" s="16" t="s">
+      <c r="E102" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F102" s="0" t="n">
@@ -5034,7 +5051,7 @@
       <c r="D103" s="0" t="n">
         <v>79.454375</v>
       </c>
-      <c r="E103" s="16" t="s">
+      <c r="E103" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F103" s="0" t="n">
@@ -5054,7 +5071,7 @@
       <c r="D104" s="0" t="n">
         <v>79.454375</v>
       </c>
-      <c r="E104" s="16" t="s">
+      <c r="E104" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F104" s="0" t="n">
@@ -5074,7 +5091,7 @@
       <c r="D105" s="0" t="n">
         <v>79.454375</v>
       </c>
-      <c r="E105" s="16" t="s">
+      <c r="E105" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F105" s="0" t="n">
@@ -5094,7 +5111,7 @@
       <c r="D106" s="0" t="n">
         <v>79.454375</v>
       </c>
-      <c r="E106" s="16" t="s">
+      <c r="E106" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F106" s="0" t="n">
@@ -5114,7 +5131,7 @@
       <c r="D107" s="0" t="n">
         <v>79.454375</v>
       </c>
-      <c r="E107" s="16" t="s">
+      <c r="E107" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F107" s="0" t="n">
@@ -5134,7 +5151,7 @@
       <c r="D108" s="0" t="n">
         <v>79.454375</v>
       </c>
-      <c r="E108" s="16" t="s">
+      <c r="E108" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F108" s="0" t="n">
@@ -5154,7 +5171,7 @@
       <c r="D109" s="0" t="n">
         <v>80.51</v>
       </c>
-      <c r="E109" s="16" t="s">
+      <c r="E109" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F109" s="0" t="n">
@@ -5174,7 +5191,7 @@
       <c r="D110" s="0" t="n">
         <v>79.454375</v>
       </c>
-      <c r="E110" s="16" t="s">
+      <c r="E110" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F110" s="0" t="n">
@@ -5194,7 +5211,7 @@
       <c r="D111" s="0" t="n">
         <v>80.59</v>
       </c>
-      <c r="E111" s="16" t="s">
+      <c r="E111" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F111" s="0" t="n">
@@ -5214,7 +5231,7 @@
       <c r="D112" s="0" t="n">
         <v>79.454375</v>
       </c>
-      <c r="E112" s="16" t="s">
+      <c r="E112" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F112" s="0" t="n">
@@ -5234,7 +5251,7 @@
       <c r="D113" s="0" t="n">
         <v>79.454375</v>
       </c>
-      <c r="E113" s="16" t="s">
+      <c r="E113" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F113" s="0" t="n">
@@ -5254,7 +5271,7 @@
       <c r="D114" s="0" t="n">
         <v>60.404375</v>
       </c>
-      <c r="E114" s="16" t="s">
+      <c r="E114" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F114" s="0" t="n">
@@ -5274,7 +5291,7 @@
       <c r="D115" s="0" t="n">
         <v>63.52</v>
       </c>
-      <c r="E115" s="16" t="s">
+      <c r="E115" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F115" s="0" t="n">
@@ -5294,7 +5311,7 @@
       <c r="D116" s="0" t="n">
         <v>60.42</v>
       </c>
-      <c r="E116" s="16" t="s">
+      <c r="E116" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F116" s="0" t="n">
@@ -5314,7 +5331,7 @@
       <c r="D117" s="0" t="n">
         <v>60.404375</v>
       </c>
-      <c r="E117" s="16" t="s">
+      <c r="E117" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F117" s="0" t="n">
@@ -5334,7 +5351,7 @@
       <c r="D118" s="0" t="n">
         <v>60.404375</v>
       </c>
-      <c r="E118" s="16" t="s">
+      <c r="E118" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F118" s="0" t="n">
@@ -5354,7 +5371,7 @@
       <c r="D119" s="0" t="n">
         <v>60.404375</v>
       </c>
-      <c r="E119" s="16" t="s">
+      <c r="E119" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F119" s="0" t="n">
@@ -5374,7 +5391,7 @@
       <c r="D120" s="0" t="n">
         <v>60.404375</v>
       </c>
-      <c r="E120" s="16" t="s">
+      <c r="E120" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F120" s="0" t="n">
@@ -5394,7 +5411,7 @@
       <c r="D121" s="0" t="n">
         <v>60.404375</v>
       </c>
-      <c r="E121" s="16" t="s">
+      <c r="E121" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F121" s="0" t="n">
@@ -5414,7 +5431,7 @@
       <c r="D122" s="0" t="n">
         <v>60.404375</v>
       </c>
-      <c r="E122" s="16" t="s">
+      <c r="E122" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F122" s="0" t="n">
@@ -5434,7 +5451,7 @@
       <c r="D123" s="0" t="n">
         <v>60.404375</v>
       </c>
-      <c r="E123" s="16" t="s">
+      <c r="E123" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F123" s="0" t="n">
@@ -5454,7 +5471,7 @@
       <c r="D124" s="0" t="n">
         <v>60.404375</v>
       </c>
-      <c r="E124" s="16" t="s">
+      <c r="E124" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F124" s="0" t="n">
@@ -5474,7 +5491,7 @@
       <c r="D125" s="0" t="n">
         <v>60.404375</v>
       </c>
-      <c r="E125" s="16" t="s">
+      <c r="E125" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F125" s="0" t="n">
@@ -5494,7 +5511,7 @@
       <c r="D126" s="0" t="n">
         <v>60.404375</v>
       </c>
-      <c r="E126" s="16" t="s">
+      <c r="E126" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F126" s="0" t="n">
@@ -5514,7 +5531,7 @@
       <c r="D127" s="0" t="n">
         <v>60.404375</v>
       </c>
-      <c r="E127" s="16" t="s">
+      <c r="E127" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F127" s="0" t="n">
@@ -5534,7 +5551,7 @@
       <c r="D128" s="0" t="n">
         <v>43.735625</v>
       </c>
-      <c r="E128" s="16" t="s">
+      <c r="E128" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F128" s="0" t="n">
@@ -5554,7 +5571,7 @@
       <c r="D129" s="0" t="n">
         <v>41.354375</v>
       </c>
-      <c r="E129" s="16" t="s">
+      <c r="E129" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F129" s="0" t="n">
@@ -5574,7 +5591,7 @@
       <c r="D130" s="0" t="n">
         <v>41.354375</v>
       </c>
-      <c r="E130" s="16" t="s">
+      <c r="E130" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F130" s="0" t="n">
@@ -5594,7 +5611,7 @@
       <c r="D131" s="0" t="n">
         <v>41.354375</v>
       </c>
-      <c r="E131" s="16" t="s">
+      <c r="E131" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F131" s="0" t="n">
@@ -5614,7 +5631,7 @@
       <c r="D132" s="0" t="n">
         <v>41.354375</v>
       </c>
-      <c r="E132" s="16" t="s">
+      <c r="E132" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F132" s="0" t="n">
@@ -5634,7 +5651,7 @@
       <c r="D133" s="0" t="n">
         <v>41.354375</v>
       </c>
-      <c r="E133" s="16" t="s">
+      <c r="E133" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F133" s="0" t="n">
@@ -5654,7 +5671,7 @@
       <c r="D134" s="0" t="n">
         <v>41.354375</v>
       </c>
-      <c r="E134" s="16" t="s">
+      <c r="E134" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F134" s="0" t="n">
@@ -5674,7 +5691,7 @@
       <c r="D135" s="0" t="n">
         <v>41.354375</v>
       </c>
-      <c r="E135" s="16" t="s">
+      <c r="E135" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F135" s="0" t="n">
@@ -5694,7 +5711,7 @@
       <c r="D136" s="0" t="n">
         <v>41.354375</v>
       </c>
-      <c r="E136" s="16" t="s">
+      <c r="E136" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F136" s="0" t="n">
@@ -5714,7 +5731,7 @@
       <c r="D137" s="0" t="n">
         <v>41.354375</v>
       </c>
-      <c r="E137" s="16" t="s">
+      <c r="E137" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F137" s="0" t="n">
@@ -5734,7 +5751,7 @@
       <c r="D138" s="0" t="n">
         <v>41.354375</v>
       </c>
-      <c r="E138" s="16" t="s">
+      <c r="E138" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F138" s="0" t="n">
@@ -5754,7 +5771,7 @@
       <c r="D139" s="0" t="n">
         <v>41.354375</v>
       </c>
-      <c r="E139" s="16" t="s">
+      <c r="E139" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F139" s="0" t="n">
@@ -5774,7 +5791,7 @@
       <c r="D140" s="0" t="n">
         <v>41.354375</v>
       </c>
-      <c r="E140" s="16" t="s">
+      <c r="E140" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F140" s="0" t="n">
@@ -5794,7 +5811,7 @@
       <c r="D141" s="0" t="n">
         <v>41.354375</v>
       </c>
-      <c r="E141" s="16" t="s">
+      <c r="E141" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F141" s="0" t="n">
@@ -5814,7 +5831,7 @@
       <c r="D142" s="0" t="n">
         <v>24.685625</v>
       </c>
-      <c r="E142" s="16" t="s">
+      <c r="E142" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F142" s="0" t="n">
@@ -5834,7 +5851,7 @@
       <c r="D143" s="0" t="n">
         <v>22.304375</v>
       </c>
-      <c r="E143" s="16" t="s">
+      <c r="E143" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F143" s="0" t="n">
@@ -5854,7 +5871,7 @@
       <c r="D144" s="0" t="n">
         <v>22.304375</v>
       </c>
-      <c r="E144" s="16" t="s">
+      <c r="E144" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F144" s="0" t="n">
@@ -5874,7 +5891,7 @@
       <c r="D145" s="0" t="n">
         <v>23.42</v>
       </c>
-      <c r="E145" s="16" t="s">
+      <c r="E145" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F145" s="0" t="n">
@@ -5894,7 +5911,7 @@
       <c r="D146" s="0" t="n">
         <v>22.304375</v>
       </c>
-      <c r="E146" s="16" t="s">
+      <c r="E146" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F146" s="0" t="n">
@@ -5914,7 +5931,7 @@
       <c r="D147" s="0" t="n">
         <v>22.304375</v>
       </c>
-      <c r="E147" s="16" t="s">
+      <c r="E147" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F147" s="0" t="n">
@@ -5934,7 +5951,7 @@
       <c r="D148" s="0" t="n">
         <v>23.32</v>
       </c>
-      <c r="E148" s="16" t="s">
+      <c r="E148" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F148" s="0" t="n">
@@ -5954,7 +5971,7 @@
       <c r="D149" s="0" t="n">
         <v>22.304375</v>
       </c>
-      <c r="E149" s="16" t="s">
+      <c r="E149" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F149" s="0" t="n">
@@ -5974,7 +5991,7 @@
       <c r="D150" s="0" t="n">
         <v>23.29</v>
       </c>
-      <c r="E150" s="16" t="s">
+      <c r="E150" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F150" s="0" t="n">
@@ -5994,7 +6011,7 @@
       <c r="D151" s="0" t="n">
         <v>22.304375</v>
       </c>
-      <c r="E151" s="16" t="s">
+      <c r="E151" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F151" s="0" t="n">
@@ -6014,7 +6031,7 @@
       <c r="D152" s="0" t="n">
         <v>22.304375</v>
       </c>
-      <c r="E152" s="16" t="s">
+      <c r="E152" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F152" s="0" t="n">
@@ -6034,7 +6051,7 @@
       <c r="D153" s="0" t="n">
         <v>22.304375</v>
       </c>
-      <c r="E153" s="16" t="s">
+      <c r="E153" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F153" s="0" t="n">
@@ -6054,7 +6071,7 @@
       <c r="D154" s="0" t="n">
         <v>22.304375</v>
       </c>
-      <c r="E154" s="16" t="s">
+      <c r="E154" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F154" s="0" t="n">
@@ -6074,7 +6091,7 @@
       <c r="D155" s="0" t="n">
         <v>19.923125</v>
       </c>
-      <c r="E155" s="16" t="s">
+      <c r="E155" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F155" s="0" t="n">
@@ -6094,7 +6111,7 @@
       <c r="D156" s="0" t="n">
         <v>3.254375</v>
       </c>
-      <c r="E156" s="16" t="s">
+      <c r="E156" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F156" s="0" t="n">
@@ -6114,7 +6131,7 @@
       <c r="D157" s="0" t="n">
         <v>3.254375</v>
       </c>
-      <c r="E157" s="16" t="s">
+      <c r="E157" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F157" s="0" t="n">
@@ -6134,7 +6151,7 @@
       <c r="D158" s="0" t="n">
         <v>3.254375</v>
       </c>
-      <c r="E158" s="16" t="s">
+      <c r="E158" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F158" s="0" t="n">
@@ -6154,7 +6171,7 @@
       <c r="D159" s="0" t="n">
         <v>3.2258</v>
       </c>
-      <c r="E159" s="16" t="s">
+      <c r="E159" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F159" s="0" t="n">
@@ -6174,7 +6191,7 @@
       <c r="D160" s="0" t="n">
         <v>3.254375</v>
       </c>
-      <c r="E160" s="16" t="s">
+      <c r="E160" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F160" s="0" t="n">
@@ -6194,7 +6211,7 @@
       <c r="D161" s="0" t="n">
         <v>4.445</v>
       </c>
-      <c r="E161" s="16" t="s">
+      <c r="E161" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F161" s="0" t="n">
@@ -6214,7 +6231,7 @@
       <c r="D162" s="0" t="n">
         <v>3.254375</v>
       </c>
-      <c r="E162" s="16" t="s">
+      <c r="E162" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F162" s="0" t="n">
@@ -6234,7 +6251,7 @@
       <c r="D163" s="0" t="n">
         <v>3.254375</v>
       </c>
-      <c r="E163" s="16" t="s">
+      <c r="E163" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F163" s="0" t="n">
@@ -6254,7 +6271,7 @@
       <c r="D164" s="0" t="n">
         <v>3.254375</v>
       </c>
-      <c r="E164" s="16" t="s">
+      <c r="E164" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F164" s="0" t="n">
@@ -6274,7 +6291,7 @@
       <c r="D165" s="0" t="n">
         <v>2.413</v>
       </c>
-      <c r="E165" s="16" t="s">
+      <c r="E165" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F165" s="0" t="n">
@@ -6294,7 +6311,7 @@
       <c r="D166" s="0" t="n">
         <v>2.032</v>
       </c>
-      <c r="E166" s="16" t="s">
+      <c r="E166" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F166" s="0" t="n">
@@ -6314,7 +6331,7 @@
       <c r="D167" s="0" t="n">
         <v>43.18</v>
       </c>
-      <c r="E167" s="16" t="s">
+      <c r="E167" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F167" s="0" t="n">
@@ -6334,7 +6351,7 @@
       <c r="D168" s="0" t="n">
         <v>87.4268</v>
       </c>
-      <c r="E168" s="16" t="s">
+      <c r="E168" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F168" s="0" t="n">
@@ -6354,7 +6371,7 @@
       <c r="D169" s="0" t="n">
         <v>91.07</v>
       </c>
-      <c r="E169" s="16" t="s">
+      <c r="E169" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F169" s="0" t="n">
@@ -6374,7 +6391,7 @@
       <c r="D170" s="0" t="n">
         <v>43.72</v>
       </c>
-      <c r="E170" s="16" t="s">
+      <c r="E170" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F170" s="0" t="n">
@@ -6394,7 +6411,7 @@
       <c r="D171" s="0" t="n">
         <v>76.82</v>
       </c>
-      <c r="E171" s="16" t="s">
+      <c r="E171" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F171" s="0" t="n">
@@ -6414,7 +6431,7 @@
       <c r="D172" s="0" t="n">
         <v>76.87</v>
       </c>
-      <c r="E172" s="16" t="s">
+      <c r="E172" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F172" s="0" t="n">
@@ -6434,7 +6451,7 @@
       <c r="D173" s="0" t="n">
         <v>75.05</v>
       </c>
-      <c r="E173" s="16" t="s">
+      <c r="E173" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F173" s="0" t="n">
@@ -6454,7 +6471,7 @@
       <c r="D174" s="0" t="n">
         <v>76.24</v>
       </c>
-      <c r="E174" s="16" t="s">
+      <c r="E174" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F174" s="0" t="n">
@@ -6474,7 +6491,7 @@
       <c r="D175" s="0" t="n">
         <v>75.82</v>
       </c>
-      <c r="E175" s="16" t="s">
+      <c r="E175" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F175" s="0" t="n">
@@ -6494,7 +6511,7 @@
       <c r="D176" s="0" t="n">
         <v>74.99</v>
       </c>
-      <c r="E176" s="16" t="s">
+      <c r="E176" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F176" s="0" t="n">
@@ -6514,7 +6531,7 @@
       <c r="D177" s="0" t="n">
         <v>75.68</v>
       </c>
-      <c r="E177" s="16" t="s">
+      <c r="E177" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F177" s="0" t="n">
@@ -6534,7 +6551,7 @@
       <c r="D178" s="0" t="n">
         <v>76.07</v>
       </c>
-      <c r="E178" s="16" t="s">
+      <c r="E178" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F178" s="0" t="n">
@@ -6554,7 +6571,7 @@
       <c r="D179" s="0" t="n">
         <v>75.18</v>
       </c>
-      <c r="E179" s="16" t="s">
+      <c r="E179" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F179" s="0" t="n">
@@ -6574,7 +6591,7 @@
       <c r="D180" s="0" t="n">
         <v>18.75</v>
       </c>
-      <c r="E180" s="16" t="s">
+      <c r="E180" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F180" s="0" t="n">
@@ -6594,7 +6611,7 @@
       <c r="D181" s="0" t="n">
         <v>19.62</v>
       </c>
-      <c r="E181" s="16" t="s">
+      <c r="E181" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F181" s="0" t="n">
@@ -6614,7 +6631,7 @@
       <c r="D182" s="0" t="n">
         <v>18.82</v>
       </c>
-      <c r="E182" s="16" t="s">
+      <c r="E182" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F182" s="0" t="n">
@@ -6634,7 +6651,7 @@
       <c r="D183" s="0" t="n">
         <v>18.8</v>
       </c>
-      <c r="E183" s="16" t="s">
+      <c r="E183" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F183" s="0" t="n">
@@ -6654,7 +6671,7 @@
       <c r="D184" s="0" t="n">
         <v>18.65</v>
       </c>
-      <c r="E184" s="16" t="s">
+      <c r="E184" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F184" s="0" t="n">
@@ -6674,7 +6691,7 @@
       <c r="D185" s="0" t="n">
         <v>19.07</v>
       </c>
-      <c r="E185" s="16" t="s">
+      <c r="E185" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F185" s="0" t="n">
@@ -6694,7 +6711,7 @@
       <c r="D186" s="0" t="n">
         <v>18.82</v>
       </c>
-      <c r="E186" s="16" t="s">
+      <c r="E186" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F186" s="0" t="n">
@@ -6714,7 +6731,7 @@
       <c r="D187" s="0" t="n">
         <v>18.8</v>
       </c>
-      <c r="E187" s="16" t="s">
+      <c r="E187" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F187" s="0" t="n">
@@ -6734,7 +6751,7 @@
       <c r="D188" s="0" t="n">
         <v>36.576</v>
       </c>
-      <c r="E188" s="16" t="s">
+      <c r="E188" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F188" s="0" t="n">
@@ -6754,7 +6771,7 @@
       <c r="D189" s="0" t="n">
         <v>53.72</v>
       </c>
-      <c r="E189" s="16" t="s">
+      <c r="E189" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F189" s="0" t="n">
@@ -6774,7 +6791,7 @@
       <c r="D190" s="0" t="n">
         <v>60.32</v>
       </c>
-      <c r="E190" s="16" t="s">
+      <c r="E190" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F190" s="0" t="n">
@@ -6794,7 +6811,7 @@
       <c r="D191" s="0" t="n">
         <v>80.1878</v>
       </c>
-      <c r="E191" s="16" t="s">
+      <c r="E191" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F191" s="0" t="n">
@@ -6814,7 +6831,7 @@
       <c r="D192" s="0" t="n">
         <v>75.28</v>
       </c>
-      <c r="E192" s="16" t="s">
+      <c r="E192" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F192" s="0" t="n">
@@ -6834,7 +6851,7 @@
       <c r="D193" s="0" t="n">
         <v>96.5708</v>
       </c>
-      <c r="E193" s="16" t="s">
+      <c r="E193" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F193" s="0" t="n">
@@ -6854,7 +6871,7 @@
       <c r="D194" s="0" t="n">
         <v>59.15</v>
       </c>
-      <c r="E194" s="16" t="s">
+      <c r="E194" s="17" t="s">
         <v>167</v>
       </c>
       <c r="F194" s="0" t="n">

</xml_diff>

<commit_message>
Fix: Inconsistencies in BOM
</commit_message>
<xml_diff>
--- a/fabrication/elecrow/CO60-PCBA-Quotation.xlsx
+++ b/fabrication/elecrow/CO60-PCBA-Quotation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="353">
   <si>
     <t>Your PCB Specification</t>
   </si>
@@ -259,13 +259,10 @@
     <t>Q1</t>
   </si>
   <si>
-    <t>FMMT493TA</t>
+    <t>FMMT495TA</t>
   </si>
   <si>
     <t>SOT-23-3</t>
-  </si>
-  <si>
-    <t>FMMT495TA</t>
   </si>
   <si>
     <t>BJT</t>
@@ -1335,6 +1332,9 @@
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
@@ -1343,9 +1343,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="3" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -3080,17 +3077,17 @@
       <c r="C10" s="14">
         <v>1.0</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="18" t="s">
         <v>81</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>82</v>
       </c>
       <c r="F10" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>83</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>84</v>
       </c>
       <c r="H10" s="11">
         <v>3.0</v>
@@ -3101,11 +3098,11 @@
       </c>
       <c r="K10" s="11"/>
       <c r="L10" t="s">
+        <v>84</v>
+      </c>
+      <c r="M10" s="12"/>
+      <c r="N10" s="19" t="s">
         <v>85</v>
-      </c>
-      <c r="M10" s="12"/>
-      <c r="N10" s="18" t="s">
-        <v>86</v>
       </c>
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
@@ -3125,7 +3122,7 @@
         <v>9.0</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="14">
         <v>68.0</v>
@@ -3136,13 +3133,13 @@
       <c r="E11" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="H11" s="20">
+      <c r="H11" s="21">
         <v>136.0</v>
       </c>
       <c r="I11" s="11"/>
@@ -3151,13 +3148,13 @@
       </c>
       <c r="K11" s="11"/>
       <c r="L11" t="s">
+        <v>89</v>
+      </c>
+      <c r="M11" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="M11" s="12" t="s">
+      <c r="N11" s="17" t="s">
         <v>91</v>
-      </c>
-      <c r="N11" s="17" t="s">
-        <v>92</v>
       </c>
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
@@ -3177,22 +3174,22 @@
         <v>10.0</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" s="14">
         <v>1.0</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="21" t="s">
-        <v>95</v>
+      <c r="F12" s="18" t="s">
+        <v>94</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H12" s="11">
         <v>2.0</v>
@@ -3203,13 +3200,13 @@
       </c>
       <c r="K12" s="11"/>
       <c r="L12" t="s">
+        <v>95</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="N12" s="17" t="s">
         <v>96</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="N12" s="17" t="s">
-        <v>97</v>
       </c>
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
@@ -3229,7 +3226,7 @@
         <v>11.0</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C13" s="14">
         <v>2.0</v>
@@ -3241,10 +3238,10 @@
         <v>39</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H13" s="11">
         <v>4.0</v>
@@ -3255,13 +3252,13 @@
       </c>
       <c r="K13" s="11"/>
       <c r="L13" t="s">
+        <v>99</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="N13" s="13" t="s">
         <v>100</v>
-      </c>
-      <c r="M13" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="N13" s="13" t="s">
-        <v>101</v>
       </c>
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
@@ -3281,22 +3278,22 @@
         <v>12.0</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" s="14">
         <v>2.0</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="21" t="s">
-        <v>104</v>
+      <c r="F14" s="18" t="s">
+        <v>103</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H14" s="11">
         <v>4.0</v>
@@ -3307,13 +3304,13 @@
       </c>
       <c r="K14" s="11"/>
       <c r="L14" t="s">
+        <v>104</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="N14" s="17" t="s">
         <v>105</v>
-      </c>
-      <c r="M14" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="N14" s="17" t="s">
-        <v>106</v>
       </c>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
@@ -3333,22 +3330,22 @@
         <v>13.0</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C15" s="14">
         <v>16.0</v>
       </c>
       <c r="D15" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="F15" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G15" s="12" t="s">
         <v>109</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>110</v>
       </c>
       <c r="H15" s="11">
         <v>64.0</v>
@@ -3359,11 +3356,11 @@
       </c>
       <c r="K15" s="11"/>
       <c r="L15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M15" s="12"/>
       <c r="N15" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
@@ -3383,22 +3380,22 @@
         <v>14.0</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C16" s="14">
         <v>1.0</v>
       </c>
       <c r="D16" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="F16" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="G16" s="12" t="s">
         <v>116</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>117</v>
       </c>
       <c r="H16" s="11">
         <v>4.0</v>
@@ -3409,11 +3406,11 @@
       </c>
       <c r="K16" s="11"/>
       <c r="L16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M16" s="12"/>
       <c r="N16" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
@@ -3433,22 +3430,22 @@
         <v>15.0</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C17" s="14">
         <v>1.0</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E17" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="F17" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="G17" s="12" t="s">
         <v>123</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>124</v>
       </c>
       <c r="H17" s="11">
         <v>5.0</v>
@@ -3459,11 +3456,11 @@
       </c>
       <c r="K17" s="11"/>
       <c r="L17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M17" s="12"/>
       <c r="N17" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
@@ -3483,22 +3480,22 @@
         <v>16.0</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C18" s="14">
         <v>1.0</v>
       </c>
       <c r="D18" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="F18" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="G18" s="12" t="s">
         <v>129</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>130</v>
       </c>
       <c r="H18" s="11">
         <v>6.0</v>
@@ -3509,11 +3506,11 @@
       </c>
       <c r="K18" s="11"/>
       <c r="L18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M18" s="12"/>
       <c r="N18" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
@@ -3533,22 +3530,22 @@
         <v>17.0</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" s="14">
         <v>1.0</v>
       </c>
       <c r="D19" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E19" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="F19" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="G19" s="13" t="s">
         <v>135</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>136</v>
       </c>
       <c r="H19" s="11">
         <v>48.0</v>
@@ -3559,11 +3556,11 @@
       </c>
       <c r="K19" s="11"/>
       <c r="L19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M19" s="12"/>
       <c r="N19" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
@@ -3583,22 +3580,22 @@
         <v>18.0</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C20" s="14">
         <v>1.0</v>
       </c>
       <c r="D20" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="F20" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>141</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>142</v>
       </c>
       <c r="H20" s="11">
         <v>5.0</v>
@@ -3609,11 +3606,11 @@
       </c>
       <c r="K20" s="11"/>
       <c r="L20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M20" s="12"/>
       <c r="N20" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
@@ -3633,22 +3630,22 @@
         <v>19.0</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C21" s="14">
         <v>1.0</v>
       </c>
       <c r="D21" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="E21" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="F21" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G21" s="12" t="s">
         <v>147</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>148</v>
       </c>
       <c r="H21" s="11">
         <v>12.0</v>
@@ -3659,11 +3656,11 @@
       </c>
       <c r="K21" s="11"/>
       <c r="L21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M21" s="12"/>
       <c r="N21" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
@@ -3683,22 +3680,22 @@
         <v>20.0</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C22" s="14">
         <v>1.0</v>
       </c>
       <c r="D22" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="F22" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="G22" s="12" t="s">
         <v>154</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>155</v>
       </c>
       <c r="H22" s="11">
         <v>4.0</v>
@@ -3709,11 +3706,11 @@
       </c>
       <c r="K22" s="11"/>
       <c r="L22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M22" s="12"/>
       <c r="N22" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
@@ -3736,7 +3733,7 @@
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
       <c r="G23" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H23" s="25">
         <f>SUM(H3:H22)</f>
@@ -3795,7 +3792,7 @@
     <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="24"/>
       <c r="B25" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C25" s="24"/>
       <c r="D25" s="24"/>
@@ -3825,7 +3822,7 @@
     <row r="26" ht="13.5" customHeight="1">
       <c r="A26" s="24"/>
       <c r="B26" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C26" s="24"/>
       <c r="D26" s="24"/>
@@ -5891,30 +5888,30 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="C1" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>163</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>164</v>
       </c>
       <c r="E1" s="28" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>166</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>167</v>
       </c>
       <c r="C2" s="31">
         <v>44.2314</v>
@@ -5923,7 +5920,7 @@
         <v>62.35</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F2" s="31">
         <v>0.0</v>
@@ -5931,10 +5928,10 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C3" s="31">
         <v>44.1814</v>
@@ -5943,7 +5940,7 @@
         <v>55.82</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F3" s="31">
         <v>180.0</v>
@@ -5951,10 +5948,10 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C4" s="31">
         <v>33.2114</v>
@@ -5963,7 +5960,7 @@
         <v>60.41</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F4" s="31">
         <v>180.0</v>
@@ -5971,10 +5968,10 @@
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" s="31">
         <v>22.2614</v>
@@ -5983,7 +5980,7 @@
         <v>55.75</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F5" s="31">
         <v>270.0</v>
@@ -5994,7 +5991,7 @@
         <v>61</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6" s="31">
         <v>20.2294</v>
@@ -6003,7 +6000,7 @@
         <v>55.75</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F6" s="31">
         <v>270.0</v>
@@ -6011,10 +6008,10 @@
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C7" s="31">
         <v>41.51376</v>
@@ -6023,7 +6020,7 @@
         <v>53.29428</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F7" s="31">
         <v>90.0</v>
@@ -6034,7 +6031,7 @@
         <v>46</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C8" s="31">
         <v>39.3314</v>
@@ -6043,7 +6040,7 @@
         <v>53.286</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F8" s="31">
         <v>90.0</v>
@@ -6051,10 +6048,10 @@
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C9" s="31">
         <v>26.8414</v>
@@ -6063,7 +6060,7 @@
         <v>46.9894</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F9" s="31">
         <v>0.0</v>
@@ -6071,10 +6068,10 @@
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C10" s="31">
         <v>41.9314</v>
@@ -6083,7 +6080,7 @@
         <v>50.62</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F10" s="31">
         <v>0.0</v>
@@ -6091,10 +6088,10 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C11" s="31">
         <v>18.3314</v>
@@ -6103,7 +6100,7 @@
         <v>63.92</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F11" s="31">
         <v>0.0</v>
@@ -6111,10 +6108,10 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="30" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C12" s="31">
         <v>15.748</v>
@@ -6123,7 +6120,7 @@
         <v>58.3946</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F12" s="31">
         <v>270.0</v>
@@ -6131,10 +6128,10 @@
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C13" s="31">
         <v>42.2214</v>
@@ -6143,7 +6140,7 @@
         <v>76.18</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F13" s="31">
         <v>270.0</v>
@@ -6151,10 +6148,10 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C14" s="31">
         <v>72.6514</v>
@@ -6163,7 +6160,7 @@
         <v>75.59</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F14" s="31">
         <v>270.0</v>
@@ -6171,10 +6168,10 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C15" s="31">
         <v>99.5014</v>
@@ -6183,7 +6180,7 @@
         <v>75.66</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F15" s="31">
         <v>270.0</v>
@@ -6191,10 +6188,10 @@
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C16" s="31">
         <v>135.0314</v>
@@ -6203,7 +6200,7 @@
         <v>76.47</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F16" s="31">
         <v>270.0</v>
@@ -6211,10 +6208,10 @@
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C17" s="31">
         <v>168.1614</v>
@@ -6223,7 +6220,7 @@
         <v>75.68</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F17" s="31">
         <v>270.0</v>
@@ -6231,10 +6228,10 @@
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C18" s="31">
         <v>202.6714</v>
@@ -6243,7 +6240,7 @@
         <v>76.03</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F18" s="31">
         <v>270.0</v>
@@ -6251,10 +6248,10 @@
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="30" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C19" s="31">
         <v>236.0514</v>
@@ -6263,7 +6260,7 @@
         <v>75.92</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F19" s="31">
         <v>270.0</v>
@@ -6271,10 +6268,10 @@
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="30" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C20" s="31">
         <v>269.4814</v>
@@ -6283,7 +6280,7 @@
         <v>75.76</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F20" s="31">
         <v>270.0</v>
@@ -6291,10 +6288,10 @@
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C21" s="31">
         <v>266.7414</v>
@@ -6303,7 +6300,7 @@
         <v>18.89</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F21" s="31">
         <v>270.0</v>
@@ -6311,10 +6308,10 @@
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C22" s="31">
         <v>236.0714</v>
@@ -6323,7 +6320,7 @@
         <v>20.07</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F22" s="31">
         <v>270.0</v>
@@ -6331,10 +6328,10 @@
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C23" s="31">
         <v>193.2214</v>
@@ -6343,7 +6340,7 @@
         <v>22.81</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F23" s="31">
         <v>90.0</v>
@@ -6351,10 +6348,10 @@
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C24" s="31">
         <v>168.9714</v>
@@ -6363,7 +6360,7 @@
         <v>20.76</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F24" s="31">
         <v>0.0</v>
@@ -6371,10 +6368,10 @@
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C25" s="31">
         <v>133.9114</v>
@@ -6383,7 +6380,7 @@
         <v>18.44</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F25" s="31">
         <v>270.0</v>
@@ -6391,10 +6388,10 @@
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="A26" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C26" s="31">
         <v>100.0314</v>
@@ -6403,7 +6400,7 @@
         <v>23.07</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F26" s="31">
         <v>180.0</v>
@@ -6411,10 +6408,10 @@
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C27" s="31">
         <v>72.0214</v>
@@ -6423,7 +6420,7 @@
         <v>18.48</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F27" s="31">
         <v>270.0</v>
@@ -6431,10 +6428,10 @@
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C28" s="31">
         <v>23.0814</v>
@@ -6443,7 +6440,7 @@
         <v>18.95</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F28" s="31">
         <v>270.0</v>
@@ -6451,10 +6448,10 @@
     </row>
     <row r="29" ht="14.25" customHeight="1">
       <c r="A29" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="B29" s="30" t="s">
         <v>193</v>
-      </c>
-      <c r="B29" s="30" t="s">
-        <v>194</v>
       </c>
       <c r="C29" s="31">
         <v>5.8674</v>
@@ -6463,7 +6460,7 @@
         <v>91.44</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F29" s="31">
         <v>180.0</v>
@@ -6471,10 +6468,10 @@
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C30" s="31">
         <v>36.522025</v>
@@ -6483,7 +6480,7 @@
         <v>86.598125</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F30" s="31">
         <v>90.0</v>
@@ -6491,10 +6488,10 @@
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C31" s="31">
         <v>55.572025</v>
@@ -6503,7 +6500,7 @@
         <v>86.598125</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F31" s="31">
         <v>90.0</v>
@@ -6511,10 +6508,10 @@
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C32" s="31">
         <v>74.7814</v>
@@ -6523,7 +6520,7 @@
         <v>88.93</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F32" s="31">
         <v>180.0</v>
@@ -6531,10 +6528,10 @@
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C33" s="31">
         <v>93.672025</v>
@@ -6543,7 +6540,7 @@
         <v>86.598125</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F33" s="31">
         <v>90.0</v>
@@ -6551,10 +6548,10 @@
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C34" s="31">
         <v>112.722025</v>
@@ -6563,7 +6560,7 @@
         <v>86.598125</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F34" s="31">
         <v>90.0</v>
@@ -6571,10 +6568,10 @@
     </row>
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C35" s="31">
         <v>131.772025</v>
@@ -6583,7 +6580,7 @@
         <v>86.598125</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F35" s="31">
         <v>90.0</v>
@@ -6591,10 +6588,10 @@
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C36" s="31">
         <v>150.822025</v>
@@ -6603,7 +6600,7 @@
         <v>86.598125</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F36" s="31">
         <v>90.0</v>
@@ -6611,10 +6608,10 @@
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C37" s="31">
         <v>169.872025</v>
@@ -6623,7 +6620,7 @@
         <v>86.598125</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F37" s="31">
         <v>90.0</v>
@@ -6631,10 +6628,10 @@
     </row>
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C38" s="31">
         <v>188.7714</v>
@@ -6643,7 +6640,7 @@
         <v>88.85</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F38" s="31">
         <v>180.0</v>
@@ -6651,10 +6648,10 @@
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="30" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C39" s="31">
         <v>207.972025</v>
@@ -6663,7 +6660,7 @@
         <v>86.598125</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F39" s="31">
         <v>90.0</v>
@@ -6671,10 +6668,10 @@
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="30" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C40" s="31">
         <v>227.022025</v>
@@ -6683,7 +6680,7 @@
         <v>86.598125</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F40" s="31">
         <v>90.0</v>
@@ -6691,10 +6688,10 @@
     </row>
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" s="30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C41" s="31">
         <v>246.072025</v>
@@ -6703,7 +6700,7 @@
         <v>86.598125</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F41" s="31">
         <v>90.0</v>
@@ -6711,10 +6708,10 @@
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C42" s="31">
         <v>265.7094</v>
@@ -6723,7 +6720,7 @@
         <v>90.17</v>
       </c>
       <c r="E42" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F42" s="31">
         <v>90.0</v>
@@ -6731,10 +6728,10 @@
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C43" s="31">
         <v>281.790775</v>
@@ -6743,7 +6740,7 @@
         <v>90.17</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F43" s="31">
         <v>90.0</v>
@@ -6751,10 +6748,10 @@
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="30" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B44" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C44" s="31">
         <v>5.565775</v>
@@ -6763,7 +6760,7 @@
         <v>71.12</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F44" s="31">
         <v>90.0</v>
@@ -6771,10 +6768,10 @@
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="30" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C45" s="31">
         <v>45.9314</v>
@@ -6783,7 +6780,7 @@
         <v>69.42</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F45" s="31">
         <v>90.0</v>
@@ -6791,10 +6788,10 @@
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="30" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B46" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C46" s="31">
         <v>65.097025</v>
@@ -6803,7 +6800,7 @@
         <v>67.548125</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F46" s="31">
         <v>90.0</v>
@@ -6811,10 +6808,10 @@
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B47" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C47" s="31">
         <v>84.147025</v>
@@ -6823,7 +6820,7 @@
         <v>67.548125</v>
       </c>
       <c r="E47" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F47" s="31">
         <v>90.0</v>
@@ -6831,10 +6828,10 @@
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="30" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C48" s="31">
         <v>103.197025</v>
@@ -6843,7 +6840,7 @@
         <v>67.548125</v>
       </c>
       <c r="E48" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F48" s="31">
         <v>90.0</v>
@@ -6851,10 +6848,10 @@
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B49" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C49" s="31">
         <v>122.247025</v>
@@ -6863,7 +6860,7 @@
         <v>67.548125</v>
       </c>
       <c r="E49" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F49" s="31">
         <v>90.0</v>
@@ -6871,10 +6868,10 @@
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B50" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C50" s="31">
         <v>141.297025</v>
@@ -6883,7 +6880,7 @@
         <v>67.548125</v>
       </c>
       <c r="E50" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F50" s="31">
         <v>90.0</v>
@@ -6891,10 +6888,10 @@
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B51" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C51" s="31">
         <v>160.347025</v>
@@ -6903,7 +6900,7 @@
         <v>67.548125</v>
       </c>
       <c r="E51" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F51" s="31">
         <v>90.0</v>
@@ -6911,10 +6908,10 @@
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="30" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B52" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C52" s="31">
         <v>179.397025</v>
@@ -6923,7 +6920,7 @@
         <v>67.548125</v>
       </c>
       <c r="E52" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F52" s="31">
         <v>90.0</v>
@@ -6931,10 +6928,10 @@
     </row>
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" s="30" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B53" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C53" s="31">
         <v>198.447025</v>
@@ -6943,7 +6940,7 @@
         <v>67.548125</v>
       </c>
       <c r="E53" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F53" s="31">
         <v>90.0</v>
@@ -6951,10 +6948,10 @@
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B54" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C54" s="31">
         <v>217.497025</v>
@@ -6963,7 +6960,7 @@
         <v>67.548125</v>
       </c>
       <c r="E54" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F54" s="31">
         <v>90.0</v>
@@ -6971,10 +6968,10 @@
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C55" s="31">
         <v>236.547025</v>
@@ -6983,7 +6980,7 @@
         <v>67.548125</v>
       </c>
       <c r="E55" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F55" s="31">
         <v>90.0</v>
@@ -6991,10 +6988,10 @@
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B56" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C56" s="31">
         <v>254.4064</v>
@@ -7003,7 +7000,7 @@
         <v>69.929375</v>
       </c>
       <c r="E56" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F56" s="31">
         <v>90.0</v>
@@ -7011,10 +7008,10 @@
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B57" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C57" s="31">
         <v>277.028275</v>
@@ -7023,7 +7020,7 @@
         <v>71.12</v>
       </c>
       <c r="E57" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F57" s="31">
         <v>90.0</v>
@@ -7031,10 +7028,10 @@
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="30" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B58" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C58" s="31">
         <v>21.0439</v>
@@ -7043,7 +7040,7 @@
         <v>42.545</v>
       </c>
       <c r="E58" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F58" s="31">
         <v>90.0</v>
@@ -7051,10 +7048,10 @@
     </row>
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" s="30" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B59" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C59" s="31">
         <v>50.809525</v>
@@ -7063,7 +7060,7 @@
         <v>48.498125</v>
       </c>
       <c r="E59" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F59" s="31">
         <v>90.0</v>
@@ -7071,10 +7068,10 @@
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="30" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B60" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C60" s="31">
         <v>69.859525</v>
@@ -7083,7 +7080,7 @@
         <v>48.498125</v>
       </c>
       <c r="E60" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F60" s="31">
         <v>90.0</v>
@@ -7091,10 +7088,10 @@
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="30" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B61" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C61" s="31">
         <v>88.909525</v>
@@ -7103,7 +7100,7 @@
         <v>48.498125</v>
       </c>
       <c r="E61" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F61" s="31">
         <v>90.0</v>
@@ -7111,10 +7108,10 @@
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" s="30" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B62" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C62" s="31">
         <v>107.959525</v>
@@ -7123,7 +7120,7 @@
         <v>48.498125</v>
       </c>
       <c r="E62" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F62" s="31">
         <v>90.0</v>
@@ -7131,10 +7128,10 @@
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="30" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C63" s="31">
         <v>110.8329</v>
@@ -7143,7 +7140,7 @@
         <v>48.5003</v>
       </c>
       <c r="E63" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F63" s="31">
         <v>90.0</v>
@@ -7151,10 +7148,10 @@
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="30" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C64" s="31">
         <v>146.059525</v>
@@ -7163,7 +7160,7 @@
         <v>48.498125</v>
       </c>
       <c r="E64" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F64" s="31">
         <v>90.0</v>
@@ -7171,10 +7168,10 @@
     </row>
     <row r="65" ht="14.25" customHeight="1">
       <c r="A65" s="30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C65" s="31">
         <v>165.109525</v>
@@ -7183,7 +7180,7 @@
         <v>48.498125</v>
       </c>
       <c r="E65" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F65" s="31">
         <v>90.0</v>
@@ -7191,10 +7188,10 @@
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="30" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B66" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C66" s="31">
         <v>184.159525</v>
@@ -7203,7 +7200,7 @@
         <v>48.498125</v>
       </c>
       <c r="E66" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F66" s="31">
         <v>90.0</v>
@@ -7211,10 +7208,10 @@
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="30" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B67" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C67" s="31">
         <v>203.209525</v>
@@ -7223,7 +7220,7 @@
         <v>48.498125</v>
       </c>
       <c r="E67" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F67" s="31">
         <v>90.0</v>
@@ -7231,10 +7228,10 @@
     </row>
     <row r="68" ht="14.25" customHeight="1">
       <c r="A68" s="30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B68" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C68" s="31">
         <v>222.259525</v>
@@ -7243,7 +7240,7 @@
         <v>48.498125</v>
       </c>
       <c r="E68" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F68" s="31">
         <v>90.0</v>
@@ -7251,10 +7248,10 @@
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="30" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B69" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C69" s="31">
         <v>241.309525</v>
@@ -7263,7 +7260,7 @@
         <v>48.498125</v>
       </c>
       <c r="E69" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F69" s="31">
         <v>90.0</v>
@@ -7271,10 +7268,10 @@
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="30" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B70" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C70" s="31">
         <v>259.1689</v>
@@ -7283,7 +7280,7 @@
         <v>54.45125</v>
       </c>
       <c r="E70" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F70" s="31">
         <v>90.0</v>
@@ -7291,10 +7288,10 @@
     </row>
     <row r="71" ht="14.25" customHeight="1">
       <c r="A71" s="30" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B71" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C71" s="31">
         <v>272.265775</v>
@@ -7303,7 +7300,7 @@
         <v>47.3075</v>
       </c>
       <c r="E71" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F71" s="31">
         <v>90.0</v>
@@ -7311,10 +7308,10 @@
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B72" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C72" s="31">
         <v>3.184525</v>
@@ -7323,7 +7320,7 @@
         <v>29.448125</v>
       </c>
       <c r="E72" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F72" s="31">
         <v>90.0</v>
@@ -7331,10 +7328,10 @@
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="30" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C73" s="31">
         <v>41.284525</v>
@@ -7343,7 +7340,7 @@
         <v>29.448125</v>
       </c>
       <c r="E73" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F73" s="31">
         <v>90.0</v>
@@ -7351,10 +7348,10 @@
     </row>
     <row r="74" ht="14.25" customHeight="1">
       <c r="A74" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C74" s="31">
         <v>60.334525</v>
@@ -7363,7 +7360,7 @@
         <v>29.448125</v>
       </c>
       <c r="E74" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F74" s="31">
         <v>90.0</v>
@@ -7371,10 +7368,10 @@
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C75" s="31">
         <v>79.384525</v>
@@ -7383,7 +7380,7 @@
         <v>29.448125</v>
       </c>
       <c r="E75" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F75" s="31">
         <v>90.0</v>
@@ -7391,10 +7388,10 @@
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B76" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C76" s="31">
         <v>98.434525</v>
@@ -7403,7 +7400,7 @@
         <v>29.448125</v>
       </c>
       <c r="E76" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F76" s="31">
         <v>90.0</v>
@@ -7411,10 +7408,10 @@
     </row>
     <row r="77" ht="14.25" customHeight="1">
       <c r="A77" s="30" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B77" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C77" s="31">
         <v>117.484525</v>
@@ -7423,7 +7420,7 @@
         <v>29.448125</v>
       </c>
       <c r="E77" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F77" s="31">
         <v>90.0</v>
@@ -7431,10 +7428,10 @@
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B78" s="32" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C78" s="31">
         <v>136.534525</v>
@@ -7443,7 +7440,7 @@
         <v>29.448125</v>
       </c>
       <c r="E78" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F78" s="31">
         <v>90.0</v>
@@ -7451,10 +7448,10 @@
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B79" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C79" s="31">
         <v>155.584525</v>
@@ -7463,7 +7460,7 @@
         <v>29.448125</v>
       </c>
       <c r="E79" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F79" s="31">
         <v>90.0</v>
@@ -7471,10 +7468,10 @@
     </row>
     <row r="80" ht="14.25" customHeight="1">
       <c r="A80" s="32" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B80" s="32" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C80" s="31">
         <v>174.634525</v>
@@ -7483,7 +7480,7 @@
         <v>29.448125</v>
       </c>
       <c r="E80" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F80" s="31">
         <v>90.0</v>
@@ -7491,10 +7488,10 @@
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="30" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B81" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C81" s="31">
         <v>193.684525</v>
@@ -7503,7 +7500,7 @@
         <v>29.448125</v>
       </c>
       <c r="E81" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F81" s="31">
         <v>90.0</v>
@@ -7511,10 +7508,10 @@
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B82" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C82" s="31">
         <v>212.734525</v>
@@ -7523,7 +7520,7 @@
         <v>29.448125</v>
       </c>
       <c r="E82" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F82" s="31">
         <v>90.0</v>
@@ -7531,10 +7528,10 @@
     </row>
     <row r="83" ht="14.25" customHeight="1">
       <c r="A83" s="30" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B83" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C83" s="31">
         <v>231.784525</v>
@@ -7543,7 +7540,7 @@
         <v>29.448125</v>
       </c>
       <c r="E83" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F83" s="31">
         <v>90.0</v>
@@ -7551,10 +7548,10 @@
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="30" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B84" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C84" s="31">
         <v>267.503275</v>
@@ -7563,7 +7560,7 @@
         <v>29.448125</v>
       </c>
       <c r="E84" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F84" s="31">
         <v>90.0</v>
@@ -7571,10 +7568,10 @@
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="30" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B85" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C85" s="31">
         <v>281.790775</v>
@@ -7583,7 +7580,7 @@
         <v>23.495</v>
       </c>
       <c r="E85" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F85" s="31">
         <v>90.0</v>
@@ -7591,10 +7588,10 @@
     </row>
     <row r="86" ht="14.25" customHeight="1">
       <c r="A86" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B86" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C86" s="31">
         <v>22.733</v>
@@ -7603,7 +7600,7 @@
         <v>13.8176</v>
       </c>
       <c r="E86" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F86" s="31">
         <v>90.0</v>
@@ -7611,10 +7608,10 @@
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="30" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B87" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C87" s="31">
         <v>46.047025</v>
@@ -7623,7 +7620,7 @@
         <v>10.398125</v>
       </c>
       <c r="E87" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F87" s="31">
         <v>90.0</v>
@@ -7631,10 +7628,10 @@
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="30" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B88" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C88" s="31">
         <v>69.859525</v>
@@ -7643,7 +7640,7 @@
         <v>10.398125</v>
       </c>
       <c r="E88" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F88" s="31">
         <v>90.0</v>
@@ -7651,10 +7648,10 @@
     </row>
     <row r="89" ht="14.25" customHeight="1">
       <c r="A89" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B89" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C89" s="31">
         <v>110.340775</v>
@@ -7663,7 +7660,7 @@
         <v>10.398125</v>
       </c>
       <c r="E89" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F89" s="31">
         <v>90.0</v>
@@ -7671,10 +7668,10 @@
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B90" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C90" s="31">
         <v>150.822025</v>
@@ -7683,7 +7680,7 @@
         <v>9.2075</v>
       </c>
       <c r="E90" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F90" s="31">
         <v>90.0</v>
@@ -7691,10 +7688,10 @@
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B91" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C91" s="31">
         <v>155.584525</v>
@@ -7703,7 +7700,7 @@
         <v>9.2075</v>
       </c>
       <c r="E91" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F91" s="31">
         <v>90.0</v>
@@ -7711,10 +7708,10 @@
     </row>
     <row r="92" ht="14.25" customHeight="1">
       <c r="A92" s="30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B92" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C92" s="31">
         <v>207.972025</v>
@@ -7723,7 +7720,7 @@
         <v>15.160625</v>
       </c>
       <c r="E92" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F92" s="31">
         <v>90.0</v>
@@ -7731,10 +7728,10 @@
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B93" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C93" s="31">
         <v>211.5439</v>
@@ -7743,7 +7740,7 @@
         <v>15.160625</v>
       </c>
       <c r="E93" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F93" s="31">
         <v>90.0</v>
@@ -7751,10 +7748,10 @@
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B94" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C94" s="31">
         <v>243.690775</v>
@@ -7763,7 +7760,7 @@
         <v>16.35125</v>
       </c>
       <c r="E94" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F94" s="31">
         <v>90.0</v>
@@ -7771,10 +7768,10 @@
     </row>
     <row r="95" ht="14.25" customHeight="1">
       <c r="A95" s="30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B95" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C95" s="31">
         <v>263.7814</v>
@@ -7783,7 +7780,7 @@
         <v>13.07</v>
       </c>
       <c r="E95" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F95" s="31">
         <v>90.0</v>
@@ -7791,10 +7788,10 @@
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B96" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C96" s="31">
         <v>281.790775</v>
@@ -7803,7 +7800,7 @@
         <v>13.97</v>
       </c>
       <c r="E96" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F96" s="31">
         <v>90.0</v>
@@ -7814,7 +7811,7 @@
         <v>73</v>
       </c>
       <c r="B97" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C97" s="31">
         <v>14.2314</v>
@@ -7823,7 +7820,7 @@
         <v>82.27</v>
       </c>
       <c r="E97" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F97" s="31">
         <v>90.0</v>
@@ -7843,7 +7840,7 @@
         <v>37.084</v>
       </c>
       <c r="E98" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F98" s="31">
         <v>270.0</v>
@@ -7851,10 +7848,10 @@
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="30" t="s">
+        <v>262</v>
+      </c>
+      <c r="B99" s="30" t="s">
         <v>263</v>
-      </c>
-      <c r="B99" s="30" t="s">
-        <v>264</v>
       </c>
       <c r="C99" s="31">
         <v>4.37515</v>
@@ -7863,7 +7860,7 @@
         <v>79.454375</v>
       </c>
       <c r="E99" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F99" s="31">
         <v>90.0</v>
@@ -7871,10 +7868,10 @@
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B100" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C100" s="31">
         <v>23.42515</v>
@@ -7883,7 +7880,7 @@
         <v>79.454375</v>
       </c>
       <c r="E100" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F100" s="31">
         <v>90.0</v>
@@ -7891,10 +7888,10 @@
     </row>
     <row r="101" ht="14.25" customHeight="1">
       <c r="A101" s="30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B101" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C101" s="31">
         <v>42.47515</v>
@@ -7903,7 +7900,7 @@
         <v>79.454375</v>
       </c>
       <c r="E101" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F101" s="31">
         <v>90.0</v>
@@ -7911,10 +7908,10 @@
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="30" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B102" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C102" s="31">
         <v>61.2714</v>
@@ -7923,7 +7920,7 @@
         <v>80.52</v>
       </c>
       <c r="E102" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F102" s="31">
         <v>90.0</v>
@@ -7931,10 +7928,10 @@
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="30" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B103" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C103" s="31">
         <v>80.57515</v>
@@ -7943,7 +7940,7 @@
         <v>79.454375</v>
       </c>
       <c r="E103" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F103" s="31">
         <v>90.0</v>
@@ -7951,10 +7948,10 @@
     </row>
     <row r="104" ht="14.25" customHeight="1">
       <c r="A104" s="30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B104" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C104" s="31">
         <v>99.62515</v>
@@ -7963,7 +7960,7 @@
         <v>79.454375</v>
       </c>
       <c r="E104" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F104" s="31">
         <v>90.0</v>
@@ -7971,10 +7968,10 @@
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B105" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C105" s="31">
         <v>118.67515</v>
@@ -7983,7 +7980,7 @@
         <v>79.454375</v>
       </c>
       <c r="E105" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F105" s="31">
         <v>90.0</v>
@@ -7991,10 +7988,10 @@
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B106" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C106" s="31">
         <v>137.72515</v>
@@ -8003,7 +8000,7 @@
         <v>79.454375</v>
       </c>
       <c r="E106" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F106" s="31">
         <v>90.0</v>
@@ -8011,10 +8008,10 @@
     </row>
     <row r="107" ht="14.25" customHeight="1">
       <c r="A107" s="30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B107" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C107" s="31">
         <v>156.77515</v>
@@ -8023,7 +8020,7 @@
         <v>79.454375</v>
       </c>
       <c r="E107" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F107" s="31">
         <v>90.0</v>
@@ -8031,10 +8028,10 @@
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="30" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B108" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C108" s="31">
         <v>175.82515</v>
@@ -8043,7 +8040,7 @@
         <v>79.454375</v>
       </c>
       <c r="E108" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F108" s="31">
         <v>90.0</v>
@@ -8051,10 +8048,10 @@
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="30" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B109" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C109" s="31">
         <v>194.1614</v>
@@ -8063,7 +8060,7 @@
         <v>80.51</v>
       </c>
       <c r="E109" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F109" s="31">
         <v>90.0</v>
@@ -8071,10 +8068,10 @@
     </row>
     <row r="110" ht="14.25" customHeight="1">
       <c r="A110" s="30" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B110" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C110" s="31">
         <v>213.92515</v>
@@ -8083,7 +8080,7 @@
         <v>79.454375</v>
       </c>
       <c r="E110" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F110" s="31">
         <v>90.0</v>
@@ -8091,10 +8088,10 @@
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B111" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C111" s="31">
         <v>232.8514</v>
@@ -8103,7 +8100,7 @@
         <v>80.59</v>
       </c>
       <c r="E111" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F111" s="31">
         <v>90.0</v>
@@ -8111,10 +8108,10 @@
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="30" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B112" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C112" s="31">
         <v>250.834525</v>
@@ -8123,7 +8120,7 @@
         <v>79.454375</v>
       </c>
       <c r="E112" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F112" s="31">
         <v>90.0</v>
@@ -8131,10 +8128,10 @@
     </row>
     <row r="113" ht="14.25" customHeight="1">
       <c r="A113" s="30" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B113" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C113" s="31">
         <v>271.07515</v>
@@ -8143,7 +8140,7 @@
         <v>79.454375</v>
       </c>
       <c r="E113" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F113" s="31">
         <v>90.0</v>
@@ -8151,10 +8148,10 @@
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="30" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B114" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C114" s="31">
         <v>9.13765</v>
@@ -8163,7 +8160,7 @@
         <v>60.404375</v>
       </c>
       <c r="E114" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F114" s="31">
         <v>90.0</v>
@@ -8171,10 +8168,10 @@
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B115" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C115" s="31">
         <v>33.0314</v>
@@ -8183,7 +8180,7 @@
         <v>63.52</v>
       </c>
       <c r="E115" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F115" s="31">
         <v>90.0</v>
@@ -8191,10 +8188,10 @@
     </row>
     <row r="116" ht="14.25" customHeight="1">
       <c r="A116" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B116" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C116" s="31">
         <v>62.1514</v>
@@ -8203,7 +8200,7 @@
         <v>60.42</v>
       </c>
       <c r="E116" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F116" s="31">
         <v>90.0</v>
@@ -8211,10 +8208,10 @@
     </row>
     <row r="117" ht="14.25" customHeight="1">
       <c r="A117" s="30" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B117" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C117" s="31">
         <v>71.05015</v>
@@ -8223,7 +8220,7 @@
         <v>60.404375</v>
       </c>
       <c r="E117" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F117" s="31">
         <v>90.0</v>
@@ -8231,10 +8228,10 @@
     </row>
     <row r="118" ht="14.25" customHeight="1">
       <c r="A118" s="30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B118" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C118" s="31">
         <v>90.10015</v>
@@ -8243,7 +8240,7 @@
         <v>60.404375</v>
       </c>
       <c r="E118" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F118" s="31">
         <v>90.0</v>
@@ -8251,10 +8248,10 @@
     </row>
     <row r="119" ht="14.25" customHeight="1">
       <c r="A119" s="30" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B119" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C119" s="31">
         <v>109.15015</v>
@@ -8263,7 +8260,7 @@
         <v>60.404375</v>
       </c>
       <c r="E119" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F119" s="31">
         <v>90.0</v>
@@ -8271,10 +8268,10 @@
     </row>
     <row r="120" ht="14.25" customHeight="1">
       <c r="A120" s="30" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B120" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C120" s="31">
         <v>128.20015</v>
@@ -8283,7 +8280,7 @@
         <v>60.404375</v>
       </c>
       <c r="E120" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F120" s="31">
         <v>90.0</v>
@@ -8291,10 +8288,10 @@
     </row>
     <row r="121" ht="14.25" customHeight="1">
       <c r="A121" s="30" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B121" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C121" s="31">
         <v>147.25015</v>
@@ -8303,7 +8300,7 @@
         <v>60.404375</v>
       </c>
       <c r="E121" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F121" s="31">
         <v>90.0</v>
@@ -8311,10 +8308,10 @@
     </row>
     <row r="122" ht="14.25" customHeight="1">
       <c r="A122" s="30" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B122" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C122" s="31">
         <v>166.30015</v>
@@ -8323,7 +8320,7 @@
         <v>60.404375</v>
       </c>
       <c r="E122" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F122" s="31">
         <v>90.0</v>
@@ -8331,10 +8328,10 @@
     </row>
     <row r="123" ht="14.25" customHeight="1">
       <c r="A123" s="30" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B123" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C123" s="31">
         <v>185.35015</v>
@@ -8343,7 +8340,7 @@
         <v>60.404375</v>
       </c>
       <c r="E123" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F123" s="31">
         <v>90.0</v>
@@ -8351,10 +8348,10 @@
     </row>
     <row r="124" ht="14.25" customHeight="1">
       <c r="A124" s="30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B124" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C124" s="31">
         <v>204.40015</v>
@@ -8363,7 +8360,7 @@
         <v>60.404375</v>
       </c>
       <c r="E124" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F124" s="31">
         <v>90.0</v>
@@ -8371,10 +8368,10 @@
     </row>
     <row r="125" ht="14.25" customHeight="1">
       <c r="A125" s="30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B125" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C125" s="31">
         <v>223.45015</v>
@@ -8383,7 +8380,7 @@
         <v>60.404375</v>
       </c>
       <c r="E125" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F125" s="31">
         <v>90.0</v>
@@ -8391,10 +8388,10 @@
     </row>
     <row r="126" ht="14.25" customHeight="1">
       <c r="A126" s="30" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B126" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C126" s="31">
         <v>242.50015</v>
@@ -8403,7 +8400,7 @@
         <v>60.404375</v>
       </c>
       <c r="E126" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F126" s="31">
         <v>90.0</v>
@@ -8411,10 +8408,10 @@
     </row>
     <row r="127" ht="14.25" customHeight="1">
       <c r="A127" s="30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B127" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C127" s="31">
         <v>266.31265</v>
@@ -8423,7 +8420,7 @@
         <v>60.404375</v>
       </c>
       <c r="E127" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F127" s="31">
         <v>90.0</v>
@@ -8431,10 +8428,10 @@
     </row>
     <row r="128" ht="14.25" customHeight="1">
       <c r="A128" s="30" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B128" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C128" s="31">
         <v>7.947025</v>
@@ -8443,7 +8440,7 @@
         <v>43.735625</v>
       </c>
       <c r="E128" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F128" s="31">
         <v>90.0</v>
@@ -8451,10 +8448,10 @@
     </row>
     <row r="129" ht="14.25" customHeight="1">
       <c r="A129" s="30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B129" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C129" s="31">
         <v>37.71265</v>
@@ -8463,7 +8460,7 @@
         <v>41.354375</v>
       </c>
       <c r="E129" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F129" s="31">
         <v>90.0</v>
@@ -8471,10 +8468,10 @@
     </row>
     <row r="130" ht="14.25" customHeight="1">
       <c r="A130" s="30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B130" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C130" s="31">
         <v>56.76265</v>
@@ -8483,7 +8480,7 @@
         <v>41.354375</v>
       </c>
       <c r="E130" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F130" s="31">
         <v>90.0</v>
@@ -8491,10 +8488,10 @@
     </row>
     <row r="131" ht="14.25" customHeight="1">
       <c r="A131" s="30" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B131" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C131" s="31">
         <v>75.81265</v>
@@ -8503,7 +8500,7 @@
         <v>41.354375</v>
       </c>
       <c r="E131" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F131" s="31">
         <v>90.0</v>
@@ -8511,10 +8508,10 @@
     </row>
     <row r="132" ht="14.25" customHeight="1">
       <c r="A132" s="30" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B132" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C132" s="31">
         <v>94.86265</v>
@@ -8523,7 +8520,7 @@
         <v>41.354375</v>
       </c>
       <c r="E132" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F132" s="31">
         <v>90.0</v>
@@ -8531,10 +8528,10 @@
     </row>
     <row r="133" ht="14.25" customHeight="1">
       <c r="A133" s="30" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B133" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C133" s="31">
         <v>113.91265</v>
@@ -8543,7 +8540,7 @@
         <v>41.354375</v>
       </c>
       <c r="E133" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F133" s="31">
         <v>90.0</v>
@@ -8551,10 +8548,10 @@
     </row>
     <row r="134" ht="14.25" customHeight="1">
       <c r="A134" s="30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B134" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C134" s="31">
         <v>132.96265</v>
@@ -8563,7 +8560,7 @@
         <v>41.354375</v>
       </c>
       <c r="E134" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F134" s="31">
         <v>90.0</v>
@@ -8571,10 +8568,10 @@
     </row>
     <row r="135" ht="14.25" customHeight="1">
       <c r="A135" s="30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B135" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C135" s="31">
         <v>152.01265</v>
@@ -8583,7 +8580,7 @@
         <v>41.354375</v>
       </c>
       <c r="E135" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F135" s="31">
         <v>90.0</v>
@@ -8591,10 +8588,10 @@
     </row>
     <row r="136" ht="14.25" customHeight="1">
       <c r="A136" s="30" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B136" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C136" s="31">
         <v>171.06265</v>
@@ -8603,7 +8600,7 @@
         <v>41.354375</v>
       </c>
       <c r="E136" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F136" s="31">
         <v>90.0</v>
@@ -8611,10 +8608,10 @@
     </row>
     <row r="137" ht="14.25" customHeight="1">
       <c r="A137" s="30" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B137" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C137" s="31">
         <v>190.11265</v>
@@ -8623,7 +8620,7 @@
         <v>41.354375</v>
       </c>
       <c r="E137" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F137" s="31">
         <v>90.0</v>
@@ -8631,10 +8628,10 @@
     </row>
     <row r="138" ht="14.25" customHeight="1">
       <c r="A138" s="30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B138" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C138" s="31">
         <v>209.16265</v>
@@ -8643,7 +8640,7 @@
         <v>41.354375</v>
       </c>
       <c r="E138" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F138" s="31">
         <v>90.0</v>
@@ -8651,10 +8648,10 @@
     </row>
     <row r="139" ht="14.25" customHeight="1">
       <c r="A139" s="30" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B139" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C139" s="31">
         <v>228.21265</v>
@@ -8663,7 +8660,7 @@
         <v>41.354375</v>
       </c>
       <c r="E139" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F139" s="31">
         <v>90.0</v>
@@ -8671,10 +8668,10 @@
     </row>
     <row r="140" ht="14.25" customHeight="1">
       <c r="A140" s="30" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B140" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C140" s="31">
         <v>247.26265</v>
@@ -8683,7 +8680,7 @@
         <v>41.354375</v>
       </c>
       <c r="E140" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F140" s="31">
         <v>90.0</v>
@@ -8691,10 +8688,10 @@
     </row>
     <row r="141" ht="14.25" customHeight="1">
       <c r="A141" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B141" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C141" s="31">
         <v>259.1689</v>
@@ -8703,7 +8700,7 @@
         <v>41.354375</v>
       </c>
       <c r="E141" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F141" s="31">
         <v>90.0</v>
@@ -8711,10 +8708,10 @@
     </row>
     <row r="142" ht="14.25" customHeight="1">
       <c r="A142" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B142" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C142" s="31">
         <v>6.7564</v>
@@ -8723,7 +8720,7 @@
         <v>24.685625</v>
       </c>
       <c r="E142" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F142" s="31">
         <v>90.0</v>
@@ -8731,10 +8728,10 @@
     </row>
     <row r="143" ht="14.25" customHeight="1">
       <c r="A143" s="30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B143" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C143" s="31">
         <v>28.18765</v>
@@ -8743,7 +8740,7 @@
         <v>22.304375</v>
       </c>
       <c r="E143" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F143" s="31">
         <v>90.0</v>
@@ -8751,10 +8748,10 @@
     </row>
     <row r="144" ht="14.25" customHeight="1">
       <c r="A144" s="30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B144" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C144" s="31">
         <v>47.23765</v>
@@ -8763,7 +8760,7 @@
         <v>22.304375</v>
       </c>
       <c r="E144" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F144" s="31">
         <v>90.0</v>
@@ -8771,10 +8768,10 @@
     </row>
     <row r="145" ht="14.25" customHeight="1">
       <c r="A145" s="30" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B145" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C145" s="31">
         <v>66.1214</v>
@@ -8783,7 +8780,7 @@
         <v>23.42</v>
       </c>
       <c r="E145" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F145" s="31">
         <v>90.0</v>
@@ -8791,10 +8788,10 @@
     </row>
     <row r="146" ht="14.25" customHeight="1">
       <c r="A146" s="30" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B146" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C146" s="31">
         <v>85.33765</v>
@@ -8803,7 +8800,7 @@
         <v>22.304375</v>
       </c>
       <c r="E146" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F146" s="31">
         <v>90.0</v>
@@ -8811,10 +8808,10 @@
     </row>
     <row r="147" ht="14.25" customHeight="1">
       <c r="A147" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B147" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C147" s="31">
         <v>104.38765</v>
@@ -8823,7 +8820,7 @@
         <v>22.304375</v>
       </c>
       <c r="E147" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F147" s="31">
         <v>90.0</v>
@@ -8831,10 +8828,10 @@
     </row>
     <row r="148" ht="14.25" customHeight="1">
       <c r="A148" s="30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B148" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C148" s="31">
         <v>123.2814</v>
@@ -8843,7 +8840,7 @@
         <v>23.32</v>
       </c>
       <c r="E148" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F148" s="31">
         <v>90.0</v>
@@ -8851,10 +8848,10 @@
     </row>
     <row r="149" ht="14.25" customHeight="1">
       <c r="A149" s="30" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B149" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C149" s="31">
         <v>142.48765</v>
@@ -8863,7 +8860,7 @@
         <v>22.304375</v>
       </c>
       <c r="E149" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F149" s="31">
         <v>90.0</v>
@@ -8871,10 +8868,10 @@
     </row>
     <row r="150" ht="14.25" customHeight="1">
       <c r="A150" s="30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B150" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C150" s="31">
         <v>161.4414</v>
@@ -8883,7 +8880,7 @@
         <v>23.29</v>
       </c>
       <c r="E150" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F150" s="31">
         <v>90.0</v>
@@ -8891,10 +8888,10 @@
     </row>
     <row r="151" ht="14.25" customHeight="1">
       <c r="A151" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B151" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C151" s="31">
         <v>180.58765</v>
@@ -8903,7 +8900,7 @@
         <v>22.304375</v>
       </c>
       <c r="E151" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F151" s="31">
         <v>90.0</v>
@@ -8911,10 +8908,10 @@
     </row>
     <row r="152" ht="14.25" customHeight="1">
       <c r="A152" s="30" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B152" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C152" s="31">
         <v>199.63765</v>
@@ -8923,7 +8920,7 @@
         <v>22.304375</v>
       </c>
       <c r="E152" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F152" s="31">
         <v>90.0</v>
@@ -8931,10 +8928,10 @@
     </row>
     <row r="153" ht="14.25" customHeight="1">
       <c r="A153" s="30" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B153" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C153" s="31">
         <v>218.68765</v>
@@ -8943,7 +8940,7 @@
         <v>22.304375</v>
       </c>
       <c r="E153" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F153" s="31">
         <v>90.0</v>
@@ -8951,10 +8948,10 @@
     </row>
     <row r="154" ht="14.25" customHeight="1">
       <c r="A154" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B154" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C154" s="31">
         <v>254.4064</v>
@@ -8963,7 +8960,7 @@
         <v>22.304375</v>
       </c>
       <c r="E154" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F154" s="31">
         <v>90.0</v>
@@ -8971,10 +8968,10 @@
     </row>
     <row r="155" ht="14.25" customHeight="1">
       <c r="A155" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B155" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C155" s="31">
         <v>275.83765</v>
@@ -8983,7 +8980,7 @@
         <v>19.923125</v>
       </c>
       <c r="E155" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F155" s="31">
         <v>0.0</v>
@@ -8991,10 +8988,10 @@
     </row>
     <row r="156" ht="14.25" customHeight="1">
       <c r="A156" s="30" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B156" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C156" s="31">
         <v>6.7564</v>
@@ -9003,7 +9000,7 @@
         <v>3.254375</v>
       </c>
       <c r="E156" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F156" s="31">
         <v>90.0</v>
@@ -9011,10 +9008,10 @@
     </row>
     <row r="157" ht="14.25" customHeight="1">
       <c r="A157" s="30" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B157" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C157" s="31">
         <v>30.5689</v>
@@ -9023,7 +9020,7 @@
         <v>3.254375</v>
       </c>
       <c r="E157" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F157" s="31">
         <v>90.0</v>
@@ -9031,10 +9028,10 @@
     </row>
     <row r="158" ht="14.25" customHeight="1">
       <c r="A158" s="32" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B158" s="32" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C158" s="31">
         <v>54.3814</v>
@@ -9043,7 +9040,7 @@
         <v>3.254375</v>
       </c>
       <c r="E158" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F158" s="31">
         <v>90.0</v>
@@ -9051,10 +9048,10 @@
     </row>
     <row r="159" ht="14.25" customHeight="1">
       <c r="A159" s="32" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B159" s="32" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C159" s="31">
         <v>117.6782</v>
@@ -9063,7 +9060,7 @@
         <v>3.2258</v>
       </c>
       <c r="E159" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F159" s="31">
         <v>90.0</v>
@@ -9071,10 +9068,10 @@
     </row>
     <row r="160" ht="14.25" customHeight="1">
       <c r="A160" s="30" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B160" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C160" s="31">
         <v>121.0564</v>
@@ -9083,7 +9080,7 @@
         <v>3.254375</v>
       </c>
       <c r="E160" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F160" s="31">
         <v>90.0</v>
@@ -9091,10 +9088,10 @@
     </row>
     <row r="161" ht="14.25" customHeight="1">
       <c r="A161" s="30" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B161" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C161" s="31">
         <v>159.1564</v>
@@ -9103,7 +9100,7 @@
         <v>4.445</v>
       </c>
       <c r="E161" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F161" s="31">
         <v>90.0</v>
@@ -9111,10 +9108,10 @@
     </row>
     <row r="162" ht="14.25" customHeight="1">
       <c r="A162" s="30" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B162" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C162" s="31">
         <v>206.7814</v>
@@ -9123,7 +9120,7 @@
         <v>3.254375</v>
       </c>
       <c r="E162" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F162" s="31">
         <v>90.0</v>
@@ -9131,10 +9128,10 @@
     </row>
     <row r="163" ht="14.25" customHeight="1">
       <c r="A163" s="30" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B163" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C163" s="31">
         <v>230.5939</v>
@@ -9143,7 +9140,7 @@
         <v>3.254375</v>
       </c>
       <c r="E163" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F163" s="31">
         <v>90.0</v>
@@ -9151,10 +9148,10 @@
     </row>
     <row r="164" ht="14.25" customHeight="1">
       <c r="A164" s="30" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B164" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C164" s="31">
         <v>234.165775</v>
@@ -9163,7 +9160,7 @@
         <v>3.254375</v>
       </c>
       <c r="E164" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F164" s="31">
         <v>90.0</v>
@@ -9171,10 +9168,10 @@
     </row>
     <row r="165" ht="14.25" customHeight="1">
       <c r="A165" s="30" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B165" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C165" s="31">
         <v>253.1364</v>
@@ -9183,7 +9180,7 @@
         <v>2.413</v>
       </c>
       <c r="E165" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F165" s="31">
         <v>270.0</v>
@@ -9191,10 +9188,10 @@
     </row>
     <row r="166" ht="14.25" customHeight="1">
       <c r="A166" s="30" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B166" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C166" s="31">
         <v>267.7414</v>
@@ -9203,7 +9200,7 @@
         <v>2.032</v>
       </c>
       <c r="E166" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F166" s="31">
         <v>90.0</v>
@@ -9211,10 +9208,10 @@
     </row>
     <row r="167" ht="14.25" customHeight="1">
       <c r="A167" s="30" t="s">
+        <v>331</v>
+      </c>
+      <c r="B167" s="30" t="s">
         <v>332</v>
-      </c>
-      <c r="B167" s="30" t="s">
-        <v>333</v>
       </c>
       <c r="C167" s="31">
         <v>29.2354</v>
@@ -9223,7 +9220,7 @@
         <v>43.18</v>
       </c>
       <c r="E167" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F167" s="31">
         <v>0.0</v>
@@ -9231,10 +9228,10 @@
     </row>
     <row r="168" ht="14.25" customHeight="1">
       <c r="A168" s="30" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B168" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C168" s="31">
         <v>12.065</v>
@@ -9243,7 +9240,7 @@
         <v>87.4268</v>
       </c>
       <c r="E168" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F168" s="31">
         <v>270.0</v>
@@ -9251,10 +9248,10 @@
     </row>
     <row r="169" ht="14.25" customHeight="1">
       <c r="A169" s="30" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B169" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C169" s="31">
         <v>26.0314</v>
@@ -9263,7 +9260,7 @@
         <v>91.07</v>
       </c>
       <c r="E169" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F169" s="31">
         <v>180.0</v>
@@ -9271,10 +9268,10 @@
     </row>
     <row r="170" ht="14.25" customHeight="1">
       <c r="A170" s="30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B170" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C170" s="31">
         <v>24.6314</v>
@@ -9283,7 +9280,7 @@
         <v>43.72</v>
       </c>
       <c r="E170" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F170" s="31">
         <v>0.0</v>
@@ -9291,10 +9288,10 @@
     </row>
     <row r="171" ht="14.25" customHeight="1">
       <c r="A171" s="30" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B171" s="30" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C171" s="31">
         <v>30.5689</v>
@@ -9303,7 +9300,7 @@
         <v>76.82</v>
       </c>
       <c r="E171" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F171" s="31">
         <v>180.0</v>
@@ -9311,10 +9308,10 @@
     </row>
     <row r="172" ht="14.25" customHeight="1">
       <c r="A172" s="30" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B172" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C172" s="31">
         <v>36.6014</v>
@@ -9323,7 +9320,7 @@
         <v>76.87</v>
       </c>
       <c r="E172" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F172" s="31">
         <v>180.0</v>
@@ -9331,10 +9328,10 @@
     </row>
     <row r="173" ht="14.25" customHeight="1">
       <c r="A173" s="30" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B173" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C173" s="31">
         <v>67.0514</v>
@@ -9343,7 +9340,7 @@
         <v>75.05</v>
       </c>
       <c r="E173" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F173" s="31">
         <v>180.0</v>
@@ -9351,10 +9348,10 @@
     </row>
     <row r="174" ht="14.25" customHeight="1">
       <c r="A174" s="30" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B174" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C174" s="31">
         <v>93.9714</v>
@@ -9363,7 +9360,7 @@
         <v>76.24</v>
       </c>
       <c r="E174" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F174" s="31">
         <v>180.0</v>
@@ -9371,10 +9368,10 @@
     </row>
     <row r="175" ht="14.25" customHeight="1">
       <c r="A175" s="30" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B175" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C175" s="31">
         <v>129.5014</v>
@@ -9383,7 +9380,7 @@
         <v>75.82</v>
       </c>
       <c r="E175" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F175" s="31">
         <v>180.0</v>
@@ -9391,10 +9388,10 @@
     </row>
     <row r="176" ht="14.25" customHeight="1">
       <c r="A176" s="30" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B176" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C176" s="31">
         <v>162.9514</v>
@@ -9403,7 +9400,7 @@
         <v>74.99</v>
       </c>
       <c r="E176" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F176" s="31">
         <v>180.0</v>
@@ -9411,10 +9408,10 @@
     </row>
     <row r="177" ht="14.25" customHeight="1">
       <c r="A177" s="30" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B177" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C177" s="31">
         <v>197.1514</v>
@@ -9423,7 +9420,7 @@
         <v>75.68</v>
       </c>
       <c r="E177" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F177" s="31">
         <v>180.0</v>
@@ -9431,10 +9428,10 @@
     </row>
     <row r="178" ht="14.25" customHeight="1">
       <c r="A178" s="30" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B178" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C178" s="31">
         <v>230.2814</v>
@@ -9443,7 +9440,7 @@
         <v>76.07</v>
       </c>
       <c r="E178" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F178" s="31">
         <v>180.0</v>
@@ -9451,10 +9448,10 @@
     </row>
     <row r="179" ht="14.25" customHeight="1">
       <c r="A179" s="30" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B179" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C179" s="31">
         <v>263.8714</v>
@@ -9463,7 +9460,7 @@
         <v>75.18</v>
       </c>
       <c r="E179" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F179" s="31">
         <v>180.0</v>
@@ -9471,10 +9468,10 @@
     </row>
     <row r="180" ht="14.25" customHeight="1">
       <c r="A180" s="30" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B180" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C180" s="31">
         <v>261.8014</v>
@@ -9483,7 +9480,7 @@
         <v>18.75</v>
       </c>
       <c r="E180" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F180" s="31">
         <v>180.0</v>
@@ -9491,10 +9488,10 @@
     </row>
     <row r="181" ht="14.25" customHeight="1">
       <c r="A181" s="30" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B181" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C181" s="31">
         <v>230.4914</v>
@@ -9503,7 +9500,7 @@
         <v>19.62</v>
       </c>
       <c r="E181" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F181" s="31">
         <v>180.0</v>
@@ -9511,10 +9508,10 @@
     </row>
     <row r="182" ht="14.25" customHeight="1">
       <c r="A182" s="30" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B182" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C182" s="31">
         <v>187.7814</v>
@@ -9523,7 +9520,7 @@
         <v>18.82</v>
       </c>
       <c r="E182" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F182" s="31">
         <v>180.0</v>
@@ -9531,10 +9528,10 @@
     </row>
     <row r="183" ht="14.25" customHeight="1">
       <c r="A183" s="30" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B183" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C183" s="31">
         <v>163.4214</v>
@@ -9543,7 +9540,7 @@
         <v>18.8</v>
       </c>
       <c r="E183" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F183" s="31">
         <v>180.0</v>
@@ -9551,10 +9548,10 @@
     </row>
     <row r="184" ht="14.25" customHeight="1">
       <c r="A184" s="30" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B184" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C184" s="31">
         <v>128.3114</v>
@@ -9563,7 +9560,7 @@
         <v>18.65</v>
       </c>
       <c r="E184" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F184" s="31">
         <v>180.0</v>
@@ -9571,10 +9568,10 @@
     </row>
     <row r="185" ht="14.25" customHeight="1">
       <c r="A185" s="30" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B185" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C185" s="31">
         <v>98.0314</v>
@@ -9583,7 +9580,7 @@
         <v>19.07</v>
       </c>
       <c r="E185" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F185" s="31">
         <v>180.0</v>
@@ -9591,10 +9588,10 @@
     </row>
     <row r="186" ht="14.25" customHeight="1">
       <c r="A186" s="30" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B186" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C186" s="31">
         <v>66.5314</v>
@@ -9603,7 +9600,7 @@
         <v>18.82</v>
       </c>
       <c r="E186" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F186" s="31">
         <v>180.0</v>
@@ -9611,10 +9608,10 @@
     </row>
     <row r="187" ht="14.25" customHeight="1">
       <c r="A187" s="30" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B187" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C187" s="31">
         <v>16.9614</v>
@@ -9623,7 +9620,7 @@
         <v>18.8</v>
       </c>
       <c r="E187" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F187" s="31">
         <v>180.0</v>
@@ -9631,10 +9628,10 @@
     </row>
     <row r="188" ht="14.25" customHeight="1">
       <c r="A188" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B188" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C188" s="31">
         <v>28.0924</v>
@@ -9643,7 +9640,7 @@
         <v>36.576</v>
       </c>
       <c r="E188" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F188" s="31">
         <v>270.0</v>
@@ -9651,10 +9648,10 @@
     </row>
     <row r="189" ht="14.25" customHeight="1">
       <c r="A189" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B189" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C189" s="31">
         <v>30.5314</v>
@@ -9663,7 +9660,7 @@
         <v>53.72</v>
       </c>
       <c r="E189" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F189" s="31">
         <v>180.0</v>
@@ -9671,10 +9668,10 @@
     </row>
     <row r="190" ht="14.25" customHeight="1">
       <c r="A190" s="30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B190" s="30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C190" s="31">
         <v>18.9314</v>
@@ -9683,7 +9680,7 @@
         <v>60.32</v>
       </c>
       <c r="E190" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F190" s="31">
         <v>270.0</v>
@@ -9691,10 +9688,10 @@
     </row>
     <row r="191" ht="14.25" customHeight="1">
       <c r="A191" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B191" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C191" s="31">
         <v>18.1102</v>
@@ -9703,7 +9700,7 @@
         <v>80.1878</v>
       </c>
       <c r="E191" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F191" s="31">
         <v>180.0</v>
@@ -9711,10 +9708,10 @@
     </row>
     <row r="192" ht="14.25" customHeight="1">
       <c r="A192" s="30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B192" s="30" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C192" s="31">
         <v>24.4014</v>
@@ -9723,7 +9720,7 @@
         <v>75.28</v>
       </c>
       <c r="E192" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F192" s="31">
         <v>0.0</v>
@@ -9731,10 +9728,10 @@
     </row>
     <row r="193" ht="14.25" customHeight="1">
       <c r="A193" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B193" s="30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C193" s="31">
         <v>18.2134</v>
@@ -9743,7 +9740,7 @@
         <v>96.5708</v>
       </c>
       <c r="E193" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F193" s="31">
         <v>0.0</v>
@@ -9751,10 +9748,10 @@
     </row>
     <row r="194" ht="14.25" customHeight="1">
       <c r="A194" s="30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B194" s="30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C194" s="31">
         <v>44.3814</v>
@@ -9763,7 +9760,7 @@
         <v>59.15</v>
       </c>
       <c r="E194" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F194" s="31">
         <v>180.0</v>

</xml_diff>